<commit_message>
Añadir carpeta eventStorming junto con el de proyecto
</commit_message>
<xml_diff>
--- a/ModelosEnriquecidos/Modelo enriquecido - Proyecto.xlsx
+++ b/ModelosEnriquecidos/Modelo enriquecido - Proyecto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Información\Downloads\DOO-working-group\ModelosEnriquecidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A1C8DC-6FF5-451F-BF9E-360484EF1ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B86BBD-8FBB-4B3E-900E-2557CFB6230B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" firstSheet="2" activeTab="2" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de dominio anémico" sheetId="61" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="155">
   <si>
     <t>Nombre</t>
   </si>
@@ -454,6 +454,63 @@
   </si>
   <si>
     <t>Este objeto de dominio contiene el estado de realización en el que puede estar una lista de tareas o una tarea</t>
+  </si>
+  <si>
+    <t>Crear</t>
+  </si>
+  <si>
+    <t>Permite crear un nuevo proyecto de gestion de tareas</t>
+  </si>
+  <si>
+    <t>Contiene los datos que tiene un proyecto</t>
+  </si>
+  <si>
+    <t>No debe existir otro proyecto con el mismo identificador</t>
+  </si>
+  <si>
+    <t>Un proyecto solo puede ser creado asociado a un equipo previamente creado</t>
+  </si>
+  <si>
+    <t>No debe haber otro proyecto asociado al equipo que crea el nuevo proyecto</t>
+  </si>
+  <si>
+    <t>La fecha de finalización debe ser posterior en linealidad de tiempo a la fecha de creación del proyecto</t>
+  </si>
+  <si>
+    <t>Existe un proyecto con el mismo identificador</t>
+  </si>
+  <si>
+    <t>Reintear indefinidamente hasta obtener un identificador que no tenga un proyecto existente</t>
+  </si>
+  <si>
+    <t>No existe el equipo que va crear dicho proyecto</t>
+  </si>
+  <si>
+    <t>Abortar y notificar que el proyecto debe ser creado baja un equipo</t>
+  </si>
+  <si>
+    <t>El equipo que intenta crear el proyecto ya tiene un proyecto existente asciado a el</t>
+  </si>
+  <si>
+    <t>Abortar y notificar que un equipo no puede tener mas de dos proyectos</t>
+  </si>
+  <si>
+    <t>La fecha que se asigno como finalización del proyecto es anterior a su fecha de creación</t>
+  </si>
+  <si>
+    <t>Abortar y notificar que la fecha de finalización debe ser posterior a haberla creado</t>
+  </si>
+  <si>
+    <t>Requerido</t>
+  </si>
+  <si>
+    <t>RequeridoOpcional</t>
+  </si>
+  <si>
+    <t>RequeridaOpcional</t>
+  </si>
+  <si>
+    <t>No requerido</t>
   </si>
 </sst>
 </file>
@@ -657,7 +714,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1021,13 +1078,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1339,6 +1502,57 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1363,59 +1577,56 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1474,13 +1685,7 @@
     <xf numFmtId="0" fontId="10" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1531,47 +1736,119 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="38" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1963,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFF4C49-240B-4036-BD62-669D42F23E67}">
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z48" sqref="Z48"/>
+    <sheetView topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W63" sqref="W63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2123,10 +2400,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD37FF8E-62F4-4178-9B49-EEA97FFC0EF4}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,77 +2413,80 @@
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="16" max="16" width="16" customWidth="1"/>
+    <col min="16" max="16" width="92.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="60.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="O1" s="120"/>
-      <c r="P1" s="120"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="121" t="str">
+      <c r="B2" s="106" t="str">
         <f>'Listado Objetos de Dominio'!$A$6</f>
         <v>Proyecto</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
-      <c r="P2" s="121"/>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+    </row>
+    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="122" t="str">
+      <c r="B3" s="107" t="str">
         <f>'Listado Objetos de Dominio'!$B$6</f>
         <v>Este objeto de dominio es la razon principal de la aplicaicion y me describe un esfuerzo general para lograr un resultado</v>
       </c>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="122"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="122"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="107"/>
+      <c r="O3" s="107"/>
+      <c r="P3" s="107"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -2255,8 +2535,24 @@
       <c r="P4" s="10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="Q4" s="220" t="str">
+        <f>A20</f>
+        <v>Crear</v>
+      </c>
+      <c r="R4" s="35" t="str">
+        <f>A20</f>
+        <v>Crear</v>
+      </c>
+      <c r="S4" s="36" t="str">
+        <f>A24</f>
+        <v>Reponsabilidad 2</v>
+      </c>
+      <c r="T4" s="2" t="str">
+        <f>A25</f>
+        <v>Reponsabilidad 3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
         <v>59</v>
       </c>
@@ -2297,8 +2593,14 @@
       <c r="P5" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="Q5" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="R5" s="23"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="31"/>
+    </row>
+    <row r="6" spans="1:20" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
@@ -2339,8 +2641,14 @@
       <c r="P6" s="7" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="Q6" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="R6" s="23"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="31"/>
+    </row>
+    <row r="7" spans="1:20" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>1</v>
       </c>
@@ -2381,8 +2689,14 @@
       <c r="P7" s="7" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q7" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="R7" s="23"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="31"/>
+    </row>
+    <row r="8" spans="1:20" ht="51" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>47</v>
       </c>
@@ -2415,8 +2729,14 @@
       <c r="P8" s="7" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q8" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="R8" s="23"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="31"/>
+    </row>
+    <row r="9" spans="1:20" ht="51" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>48</v>
       </c>
@@ -2449,8 +2769,14 @@
       <c r="P9" s="7" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="R9" s="23"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="31"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>134</v>
       </c>
@@ -2471,8 +2797,14 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="7"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="R10" s="23"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="31"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>133</v>
       </c>
@@ -2493,8 +2825,14 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="7"/>
-    </row>
-    <row r="12" spans="1:16" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="Q11" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="R11" s="23"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="31"/>
+    </row>
+    <row r="12" spans="1:20" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>90</v>
       </c>
@@ -2539,8 +2877,14 @@
       <c r="P12" s="7" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q12" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="R12" s="23"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="31"/>
+    </row>
+    <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2558,12 +2902,12 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="123" t="s">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="124"/>
-      <c r="C14" s="125"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="110"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2578,7 +2922,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>21</v>
       </c>
@@ -2602,7 +2946,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="103"/>
@@ -2620,7 +2964,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2638,41 +2982,45 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="126" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="127"/>
-      <c r="C18" s="127" t="s">
+      <c r="B18" s="112"/>
+      <c r="C18" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="127"/>
-      <c r="E18" s="127"/>
-      <c r="F18" s="127"/>
-      <c r="G18" s="127" t="s">
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="127"/>
-      <c r="I18" s="127"/>
-      <c r="J18" s="127" t="s">
+      <c r="H18" s="112"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="K18" s="127"/>
-      <c r="L18" s="127"/>
-      <c r="M18" s="127"/>
-      <c r="N18" s="127"/>
-      <c r="O18" s="127" t="s">
+      <c r="K18" s="112"/>
+      <c r="L18" s="112"/>
+      <c r="M18" s="112"/>
+      <c r="N18" s="112"/>
+      <c r="O18" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="P18" s="127"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="128"/>
-      <c r="B19" s="129"/>
-      <c r="C19" s="129"/>
-      <c r="D19" s="129"/>
-      <c r="E19" s="129"/>
-      <c r="F19" s="129"/>
+      <c r="P18" s="112"/>
+      <c r="Q18" s="112" t="s">
+        <v>27</v>
+      </c>
+      <c r="R18" s="130"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="113"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="114"/>
+      <c r="D19" s="114"/>
+      <c r="E19" s="114"/>
+      <c r="F19" s="114"/>
       <c r="G19" s="19" t="s">
         <v>28</v>
       </c>
@@ -2685,101 +3033,232 @@
       <c r="J19" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K19" s="129" t="s">
+      <c r="K19" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="L19" s="129"/>
-      <c r="M19" s="129"/>
-      <c r="N19" s="129"/>
+      <c r="L19" s="114"/>
+      <c r="M19" s="114"/>
+      <c r="N19" s="114"/>
       <c r="O19" s="19" t="s">
         <v>30</v>
       </c>
       <c r="P19" s="19" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="113" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="114"/>
-      <c r="C20" s="115"/>
-      <c r="D20" s="115"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="115"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="115"/>
-      <c r="L20" s="115"/>
-      <c r="M20" s="115"/>
-      <c r="N20" s="115"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="116" t="s">
+      <c r="Q19" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="R19" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="196" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" s="197"/>
+      <c r="C20" s="202" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="203"/>
+      <c r="E20" s="203"/>
+      <c r="F20" s="204"/>
+      <c r="G20" s="211" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" s="214" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" s="217" t="s">
+        <v>138</v>
+      </c>
+      <c r="J20" s="214"/>
+      <c r="K20" s="202"/>
+      <c r="L20" s="203"/>
+      <c r="M20" s="203"/>
+      <c r="N20" s="204"/>
+      <c r="O20" s="20">
+        <v>1</v>
+      </c>
+      <c r="P20" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q20" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="R20" s="195" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="198"/>
+      <c r="B21" s="199"/>
+      <c r="C21" s="205"/>
+      <c r="D21" s="206"/>
+      <c r="E21" s="206"/>
+      <c r="F21" s="207"/>
+      <c r="G21" s="212"/>
+      <c r="H21" s="215"/>
+      <c r="I21" s="218"/>
+      <c r="J21" s="215"/>
+      <c r="K21" s="205"/>
+      <c r="L21" s="206"/>
+      <c r="M21" s="206"/>
+      <c r="N21" s="207"/>
+      <c r="O21" s="20">
+        <v>2</v>
+      </c>
+      <c r="P21" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q21" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="R21" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="198"/>
+      <c r="B22" s="199"/>
+      <c r="C22" s="205"/>
+      <c r="D22" s="206"/>
+      <c r="E22" s="206"/>
+      <c r="F22" s="207"/>
+      <c r="G22" s="212"/>
+      <c r="H22" s="215"/>
+      <c r="I22" s="218"/>
+      <c r="J22" s="215"/>
+      <c r="K22" s="205"/>
+      <c r="L22" s="206"/>
+      <c r="M22" s="206"/>
+      <c r="N22" s="207"/>
+      <c r="O22" s="20">
+        <v>3</v>
+      </c>
+      <c r="P22" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q22" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="R22" s="22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="200"/>
+      <c r="B23" s="201"/>
+      <c r="C23" s="208"/>
+      <c r="D23" s="209"/>
+      <c r="E23" s="209"/>
+      <c r="F23" s="210"/>
+      <c r="G23" s="213"/>
+      <c r="H23" s="216"/>
+      <c r="I23" s="219"/>
+      <c r="J23" s="216"/>
+      <c r="K23" s="208"/>
+      <c r="L23" s="209"/>
+      <c r="M23" s="209"/>
+      <c r="N23" s="210"/>
+      <c r="O23" s="20">
+        <v>4</v>
+      </c>
+      <c r="P23" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q23" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="R23" s="22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="117"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="119"/>
-      <c r="L21" s="119"/>
-      <c r="M21" s="119"/>
-      <c r="N21" s="119"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="24"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="105" t="s">
+      <c r="B24" s="119"/>
+      <c r="C24" s="120"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="120"/>
+      <c r="F24" s="120"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="121"/>
+      <c r="L24" s="121"/>
+      <c r="M24" s="121"/>
+      <c r="N24" s="121"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="106"/>
-      <c r="C22" s="107"/>
-      <c r="D22" s="107"/>
-      <c r="E22" s="107"/>
-      <c r="F22" s="107"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="108"/>
-      <c r="L22" s="108"/>
-      <c r="M22" s="108"/>
-      <c r="N22" s="108"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="29"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="109" t="s">
+      <c r="B25" s="123"/>
+      <c r="C25" s="124"/>
+      <c r="D25" s="124"/>
+      <c r="E25" s="124"/>
+      <c r="F25" s="124"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="125"/>
+      <c r="L25" s="125"/>
+      <c r="M25" s="125"/>
+      <c r="N25" s="125"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="110"/>
-      <c r="C23" s="111"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="111"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="112"/>
-      <c r="L23" s="112"/>
-      <c r="M23" s="112"/>
-      <c r="N23" s="112"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="32"/>
+      <c r="B26" s="127"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="129"/>
+      <c r="L26" s="129"/>
+      <c r="M26" s="129"/>
+      <c r="N26" s="129"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="27">
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="A20:B23"/>
+    <mergeCell ref="C20:F23"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="K20:N23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="K24:N24"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
@@ -2790,29 +3269,22 @@
     <mergeCell ref="J18:N18"/>
     <mergeCell ref="O18:P18"/>
     <mergeCell ref="K19:N19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="K23:N23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{47778F30-7A22-4070-8157-D398D2A3CE0F}"/>
-    <hyperlink ref="H23" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{D3F545D0-6E58-49FD-B848-5263BA70789A}"/>
-    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{D4226CCC-5E80-4BCE-91C7-8796296A1724}"/>
-    <hyperlink ref="A20:B20" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{E3DD67C7-4FB8-4BCE-94B1-30DBE2583F2C}"/>
-    <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{077D1BD0-B2E1-4C60-BE34-F7EFEE0BE80F}"/>
+    <hyperlink ref="H26" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{D3F545D0-6E58-49FD-B848-5263BA70789A}"/>
+    <hyperlink ref="A24:B24" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{D4226CCC-5E80-4BCE-91C7-8796296A1724}"/>
+    <hyperlink ref="A26:B26" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{077D1BD0-B2E1-4C60-BE34-F7EFEE0BE80F}"/>
     <hyperlink ref="A1:P1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{A01559FD-0C7C-4112-A809-F49F4DACD93C}"/>
-    <hyperlink ref="A22:B22" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{8552B757-8DC3-490E-A26C-09AD5D9DDA62}"/>
+    <hyperlink ref="A25:B25" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{8552B757-8DC3-490E-A26C-09AD5D9DDA62}"/>
     <hyperlink ref="B10" location="ObjetoDominio_Participante!A1" display="Participante" xr:uid="{65BE0D2A-5223-4BAE-A78D-FEF01705AAE1}"/>
     <hyperlink ref="B11" location="ObjetoDominio_ListaTarea!A1" display="ListaTareas" xr:uid="{4B321ACB-9E6C-44EE-95C8-0229FF27DA74}"/>
+    <hyperlink ref="H20" location="ObjetoDominio_Proyectos!A1" display="Proyecto" xr:uid="{40CC0287-00F3-4ABE-A060-C8487E637CC8}"/>
+    <hyperlink ref="R4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{AB371578-E9ED-4E92-AAAC-6A9DAB3728CA}"/>
+    <hyperlink ref="S4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{A18C8F13-1F14-44DB-A0ED-D45BA28B04B6}"/>
+    <hyperlink ref="T4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{266F3904-D4CD-4A7F-9A48-5F780CAB7CD0}"/>
+    <hyperlink ref="Q4" location="ObjetoDominio_Proyectos!A20" display="ObjetoDominio_Proyectos!A20" xr:uid="{988D7633-97BF-4994-82C5-0CC5828A6983}"/>
+    <hyperlink ref="A20:B23" location="ObjetoDominio_Proyectos!Q4" display="Crear" xr:uid="{FD470CAC-8EBE-4274-9F01-02F0EB28E4C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2823,7 +3295,7 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="Q17" sqref="Q17:R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2853,70 +3325,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="O1" s="120"/>
-      <c r="P1" s="120"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="121" t="str">
+      <c r="B2" s="106" t="str">
         <f>'Listado Objetos de Dominio'!$A$2</f>
         <v>ListaTareas</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
-      <c r="P2" s="121"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="122" t="str">
+      <c r="B3" s="107" t="str">
         <f>'Listado Objetos de Dominio'!$B$2</f>
         <v xml:space="preserve">Este objeto de dominio contiene  informacion de las listas de trabajo que tienen los proyectos </v>
       </c>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="122"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="122"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="107"/>
+      <c r="O3" s="107"/>
+      <c r="P3" s="107"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2969,7 +3441,7 @@
       </c>
       <c r="Q4" s="37" t="str">
         <f>A19</f>
-        <v>Reponsabilidad 1</v>
+        <v>Crear</v>
       </c>
       <c r="R4" s="35" t="str">
         <f>A20</f>
@@ -3288,11 +3760,11 @@
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="123" t="s">
+      <c r="A13" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="124"/>
-      <c r="C13" s="125"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="110"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
@@ -3311,44 +3783,44 @@
       <c r="C15" s="38"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="126" t="s">
+      <c r="A17" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="127"/>
-      <c r="C17" s="127" t="s">
+      <c r="B17" s="112"/>
+      <c r="C17" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="127"/>
-      <c r="E17" s="127"/>
-      <c r="F17" s="127"/>
-      <c r="G17" s="127" t="s">
+      <c r="D17" s="112"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="127"/>
-      <c r="I17" s="127"/>
-      <c r="J17" s="127" t="s">
+      <c r="H17" s="112"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="K17" s="127"/>
-      <c r="L17" s="127"/>
-      <c r="M17" s="127"/>
-      <c r="N17" s="127"/>
-      <c r="O17" s="127" t="s">
+      <c r="K17" s="112"/>
+      <c r="L17" s="112"/>
+      <c r="M17" s="112"/>
+      <c r="N17" s="112"/>
+      <c r="O17" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="127"/>
-      <c r="Q17" s="127" t="s">
+      <c r="P17" s="112"/>
+      <c r="Q17" s="112" t="s">
         <v>27</v>
       </c>
       <c r="R17" s="130"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="128"/>
-      <c r="B18" s="129"/>
-      <c r="C18" s="129"/>
-      <c r="D18" s="129"/>
-      <c r="E18" s="129"/>
-      <c r="F18" s="129"/>
+      <c r="A18" s="113"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="114"/>
+      <c r="E18" s="114"/>
+      <c r="F18" s="114"/>
       <c r="G18" s="19" t="s">
         <v>28</v>
       </c>
@@ -3361,12 +3833,12 @@
       <c r="J18" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K18" s="129" t="s">
+      <c r="K18" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="L18" s="129"/>
-      <c r="M18" s="129"/>
-      <c r="N18" s="129"/>
+      <c r="L18" s="114"/>
+      <c r="M18" s="114"/>
+      <c r="N18" s="114"/>
       <c r="O18" s="19" t="s">
         <v>30</v>
       </c>
@@ -3380,89 +3852,95 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="113" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="114"/>
-      <c r="C19" s="115"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="115"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="21"/>
+    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="115" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="116"/>
+      <c r="C19" s="183" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="184"/>
+      <c r="E19" s="184"/>
+      <c r="F19" s="185"/>
+      <c r="G19" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>126</v>
+      </c>
       <c r="I19" s="22"/>
       <c r="J19" s="21"/>
-      <c r="K19" s="115"/>
-      <c r="L19" s="115"/>
-      <c r="M19" s="115"/>
-      <c r="N19" s="115"/>
+      <c r="K19" s="117"/>
+      <c r="L19" s="117"/>
+      <c r="M19" s="117"/>
+      <c r="N19" s="117"/>
       <c r="O19" s="20"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="26"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="116" t="s">
+      <c r="A20" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="118"/>
-      <c r="D20" s="118"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="118"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="186"/>
+      <c r="D20" s="187"/>
+      <c r="E20" s="187"/>
+      <c r="F20" s="188"/>
       <c r="G20" s="46"/>
       <c r="H20" s="44"/>
       <c r="I20" s="45"/>
       <c r="J20" s="39"/>
-      <c r="K20" s="119"/>
-      <c r="L20" s="119"/>
-      <c r="M20" s="119"/>
-      <c r="N20" s="119"/>
+      <c r="K20" s="121"/>
+      <c r="L20" s="121"/>
+      <c r="M20" s="121"/>
+      <c r="N20" s="121"/>
       <c r="O20" s="23"/>
       <c r="P20" s="24"/>
       <c r="Q20" s="24"/>
       <c r="R20" s="27"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="105" t="s">
+      <c r="A21" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="106"/>
-      <c r="C21" s="107"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107"/>
+      <c r="B21" s="123"/>
+      <c r="C21" s="189"/>
+      <c r="D21" s="190"/>
+      <c r="E21" s="190"/>
+      <c r="F21" s="191"/>
       <c r="G21" s="42"/>
       <c r="H21" s="40"/>
       <c r="I21" s="41"/>
       <c r="J21" s="43"/>
-      <c r="K21" s="108"/>
-      <c r="L21" s="108"/>
-      <c r="M21" s="108"/>
-      <c r="N21" s="108"/>
+      <c r="K21" s="125"/>
+      <c r="L21" s="125"/>
+      <c r="M21" s="125"/>
+      <c r="N21" s="125"/>
       <c r="O21" s="28"/>
       <c r="P21" s="29"/>
       <c r="Q21" s="29"/>
       <c r="R21" s="30"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="109" t="s">
+      <c r="A22" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="110"/>
-      <c r="C22" s="111"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="111"/>
-      <c r="F22" s="111"/>
+      <c r="B22" s="127"/>
+      <c r="C22" s="192"/>
+      <c r="D22" s="193"/>
+      <c r="E22" s="193"/>
+      <c r="F22" s="194"/>
       <c r="G22" s="48"/>
       <c r="H22" s="49"/>
       <c r="I22" s="47"/>
       <c r="J22" s="48"/>
-      <c r="K22" s="112"/>
-      <c r="L22" s="112"/>
-      <c r="M22" s="112"/>
-      <c r="N22" s="112"/>
+      <c r="K22" s="129"/>
+      <c r="L22" s="129"/>
+      <c r="M22" s="129"/>
+      <c r="N22" s="129"/>
       <c r="O22" s="31"/>
       <c r="P22" s="32"/>
       <c r="Q22" s="32"/>
@@ -3470,6 +3948,20 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="K19:N19"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
@@ -3479,20 +3971,6 @@
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="J17:N17"/>
     <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:F20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{F92E8141-0BAA-4CFF-A2AA-790349ADA214}"/>
@@ -3506,6 +3984,7 @@
     <hyperlink ref="Q4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{F66CECC3-2EE1-49F8-9E57-39E041254432}"/>
     <hyperlink ref="A1:P1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{BAD90D86-7311-49B0-A802-02D69BE204D5}"/>
     <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{1BF344DA-00DC-4E3D-9686-31B0C99A39F5}"/>
+    <hyperlink ref="H19" location="ObjetoDominio_Proyectos!A1" display="Proyecto" xr:uid="{2B76A8D7-C542-415D-85CD-908C47C772FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3548,70 +4027,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="O1" s="120"/>
-      <c r="P1" s="120"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="121" t="str">
+      <c r="B2" s="106" t="str">
         <f>'Listado Objetos de Dominio'!$A$3</f>
         <v>Participante</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
-      <c r="P2" s="121"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="122" t="str">
+      <c r="B3" s="107" t="str">
         <f>'Listado Objetos de Dominio'!$B$3</f>
         <v xml:space="preserve">Este objeto de dominio me da la informacion de la persona que esta vinculada al proyecto </v>
       </c>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="122"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="122"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="107"/>
+      <c r="O3" s="107"/>
+      <c r="P3" s="107"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -3911,11 +4390,11 @@
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="123" t="s">
+      <c r="A11" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="124"/>
-      <c r="C11" s="125"/>
+      <c r="B11" s="109"/>
+      <c r="C11" s="110"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
@@ -3934,44 +4413,44 @@
       <c r="C13" s="38"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="126" t="s">
+      <c r="A15" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="127"/>
-      <c r="C15" s="127" t="s">
+      <c r="B15" s="112"/>
+      <c r="C15" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="127"/>
-      <c r="E15" s="127"/>
-      <c r="F15" s="127"/>
-      <c r="G15" s="127" t="s">
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="127"/>
-      <c r="I15" s="127"/>
-      <c r="J15" s="127" t="s">
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="127"/>
-      <c r="L15" s="127"/>
-      <c r="M15" s="127"/>
-      <c r="N15" s="127"/>
-      <c r="O15" s="127" t="s">
+      <c r="K15" s="112"/>
+      <c r="L15" s="112"/>
+      <c r="M15" s="112"/>
+      <c r="N15" s="112"/>
+      <c r="O15" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="127"/>
-      <c r="Q15" s="127" t="s">
+      <c r="P15" s="112"/>
+      <c r="Q15" s="112" t="s">
         <v>27</v>
       </c>
       <c r="R15" s="130"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="128"/>
-      <c r="B16" s="129"/>
-      <c r="C16" s="129"/>
-      <c r="D16" s="129"/>
-      <c r="E16" s="129"/>
-      <c r="F16" s="129"/>
+      <c r="A16" s="113"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="114"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="114"/>
       <c r="G16" s="19" t="s">
         <v>28</v>
       </c>
@@ -3984,12 +4463,12 @@
       <c r="J16" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="129" t="s">
+      <c r="K16" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="L16" s="129"/>
-      <c r="M16" s="129"/>
-      <c r="N16" s="129"/>
+      <c r="L16" s="114"/>
+      <c r="M16" s="114"/>
+      <c r="N16" s="114"/>
       <c r="O16" s="19" t="s">
         <v>30</v>
       </c>
@@ -4004,88 +4483,88 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="113" t="s">
+      <c r="A17" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="114"/>
-      <c r="C17" s="115"/>
-      <c r="D17" s="115"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="115"/>
+      <c r="B17" s="116"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
       <c r="G17" s="20"/>
       <c r="H17" s="21"/>
       <c r="I17" s="22"/>
       <c r="J17" s="21"/>
-      <c r="K17" s="115"/>
-      <c r="L17" s="115"/>
-      <c r="M17" s="115"/>
-      <c r="N17" s="115"/>
+      <c r="K17" s="117"/>
+      <c r="L17" s="117"/>
+      <c r="M17" s="117"/>
+      <c r="N17" s="117"/>
       <c r="O17" s="20"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="26"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="116" t="s">
+      <c r="A18" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="117"/>
-      <c r="C18" s="118"/>
-      <c r="D18" s="118"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
+      <c r="B18" s="119"/>
+      <c r="C18" s="120"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
       <c r="G18" s="46"/>
       <c r="H18" s="44"/>
       <c r="I18" s="45"/>
       <c r="J18" s="39"/>
-      <c r="K18" s="119"/>
-      <c r="L18" s="119"/>
-      <c r="M18" s="119"/>
-      <c r="N18" s="119"/>
+      <c r="K18" s="121"/>
+      <c r="L18" s="121"/>
+      <c r="M18" s="121"/>
+      <c r="N18" s="121"/>
       <c r="O18" s="23"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
       <c r="R18" s="27"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="105" t="s">
+      <c r="A19" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="106"/>
-      <c r="C19" s="107"/>
-      <c r="D19" s="107"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="107"/>
+      <c r="B19" s="123"/>
+      <c r="C19" s="124"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="124"/>
       <c r="G19" s="42"/>
       <c r="H19" s="40"/>
       <c r="I19" s="41"/>
       <c r="J19" s="43"/>
-      <c r="K19" s="108"/>
-      <c r="L19" s="108"/>
-      <c r="M19" s="108"/>
-      <c r="N19" s="108"/>
+      <c r="K19" s="125"/>
+      <c r="L19" s="125"/>
+      <c r="M19" s="125"/>
+      <c r="N19" s="125"/>
       <c r="O19" s="28"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="29"/>
       <c r="R19" s="30"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="109" t="s">
+      <c r="A20" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="110"/>
-      <c r="C20" s="111"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="111"/>
-      <c r="F20" s="111"/>
+      <c r="B20" s="127"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="128"/>
+      <c r="F20" s="128"/>
       <c r="G20" s="48"/>
       <c r="H20" s="49"/>
       <c r="I20" s="47"/>
       <c r="J20" s="48"/>
-      <c r="K20" s="112"/>
-      <c r="L20" s="112"/>
-      <c r="M20" s="112"/>
-      <c r="N20" s="112"/>
+      <c r="K20" s="129"/>
+      <c r="L20" s="129"/>
+      <c r="M20" s="129"/>
+      <c r="N20" s="129"/>
       <c r="O20" s="31"/>
       <c r="P20" s="32"/>
       <c r="Q20" s="32"/>
@@ -4093,17 +4572,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="K17:N17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="K18:N18"/>
@@ -4116,6 +4584,17 @@
     <mergeCell ref="G15:I15"/>
     <mergeCell ref="J15:N15"/>
     <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="K20:N20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{BD3FFCC5-4B44-4838-A36D-76DB08190487}"/>
@@ -4156,24 +4635,24 @@
       <c r="A1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="172" t="str">
+      <c r="B1" s="136" t="str">
         <f>'Listado Objetos de Dominio'!$A$7</f>
         <v>MetricaProyecto</v>
       </c>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="173"/>
-      <c r="O1" s="173"/>
-      <c r="P1" s="174"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="137"/>
+      <c r="N1" s="137"/>
+      <c r="O1" s="137"/>
+      <c r="P1" s="138"/>
       <c r="Q1" s="57"/>
       <c r="R1" s="57"/>
       <c r="S1" s="57"/>
@@ -4183,24 +4662,24 @@
       <c r="A2" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="169" t="str">
+      <c r="B2" s="133" t="str">
         <f>'Listado Objetos de Dominio'!$B$7</f>
         <v>Objeto de dominio que contiene los datos necesarios para realizar el analisis estadistico a proyecto</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
-      <c r="P2" s="171"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
+      <c r="O2" s="134"/>
+      <c r="P2" s="135"/>
       <c r="Q2" s="57"/>
       <c r="R2" s="57"/>
       <c r="S2" s="57"/>
@@ -4567,11 +5046,11 @@
       <c r="T10" s="57"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="139" t="s">
+      <c r="A11" s="155" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="140"/>
-      <c r="C11" s="141"/>
+      <c r="B11" s="156"/>
+      <c r="C11" s="157"/>
       <c r="D11" s="57"/>
       <c r="E11" s="57"/>
       <c r="F11" s="57"/>
@@ -4673,46 +5152,46 @@
       <c r="T14" s="57"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="142" t="s">
+      <c r="A15" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="143"/>
-      <c r="C15" s="146" t="s">
+      <c r="B15" s="159"/>
+      <c r="C15" s="162" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="147"/>
-      <c r="E15" s="147"/>
-      <c r="F15" s="143"/>
-      <c r="G15" s="150" t="s">
+      <c r="D15" s="163"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="159"/>
+      <c r="G15" s="131" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="151"/>
-      <c r="I15" s="152"/>
-      <c r="J15" s="150" t="s">
+      <c r="H15" s="166"/>
+      <c r="I15" s="132"/>
+      <c r="J15" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="151"/>
-      <c r="L15" s="151"/>
-      <c r="M15" s="151"/>
-      <c r="N15" s="152"/>
-      <c r="O15" s="150" t="s">
+      <c r="K15" s="166"/>
+      <c r="L15" s="166"/>
+      <c r="M15" s="166"/>
+      <c r="N15" s="132"/>
+      <c r="O15" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="152"/>
-      <c r="Q15" s="150" t="s">
+      <c r="P15" s="132"/>
+      <c r="Q15" s="131" t="s">
         <v>27</v>
       </c>
-      <c r="R15" s="152"/>
+      <c r="R15" s="132"/>
       <c r="S15" s="57"/>
       <c r="T15" s="57"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="144"/>
-      <c r="B16" s="145"/>
-      <c r="C16" s="148"/>
-      <c r="D16" s="149"/>
-      <c r="E16" s="149"/>
-      <c r="F16" s="145"/>
+      <c r="A16" s="160"/>
+      <c r="B16" s="161"/>
+      <c r="C16" s="164"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="161"/>
       <c r="G16" s="79" t="s">
         <v>28</v>
       </c>
@@ -4725,12 +5204,12 @@
       <c r="J16" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="161" t="s">
+      <c r="K16" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="L16" s="162"/>
-      <c r="M16" s="162"/>
-      <c r="N16" s="163"/>
+      <c r="L16" s="176"/>
+      <c r="M16" s="176"/>
+      <c r="N16" s="177"/>
       <c r="O16" s="79" t="s">
         <v>30</v>
       </c>
@@ -4747,22 +5226,22 @@
       <c r="T16" s="57"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="164" t="s">
+      <c r="A17" s="178" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="165"/>
-      <c r="C17" s="166"/>
-      <c r="D17" s="167"/>
-      <c r="E17" s="167"/>
-      <c r="F17" s="168"/>
+      <c r="B17" s="179"/>
+      <c r="C17" s="180"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="181"/>
+      <c r="F17" s="182"/>
       <c r="G17" s="81"/>
       <c r="H17" s="82"/>
       <c r="I17" s="83"/>
       <c r="J17" s="82"/>
-      <c r="K17" s="166"/>
-      <c r="L17" s="167"/>
-      <c r="M17" s="167"/>
-      <c r="N17" s="168"/>
+      <c r="K17" s="180"/>
+      <c r="L17" s="181"/>
+      <c r="M17" s="181"/>
+      <c r="N17" s="182"/>
       <c r="O17" s="81"/>
       <c r="P17" s="81"/>
       <c r="Q17" s="81"/>
@@ -4771,22 +5250,22 @@
       <c r="T17" s="57"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="175" t="s">
+      <c r="A18" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="176"/>
-      <c r="C18" s="177"/>
-      <c r="D18" s="178"/>
-      <c r="E18" s="178"/>
-      <c r="F18" s="179"/>
+      <c r="B18" s="140"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="142"/>
+      <c r="E18" s="142"/>
+      <c r="F18" s="143"/>
       <c r="G18" s="85"/>
       <c r="H18" s="86"/>
       <c r="I18" s="87"/>
       <c r="J18" s="88"/>
-      <c r="K18" s="180"/>
-      <c r="L18" s="181"/>
-      <c r="M18" s="181"/>
-      <c r="N18" s="182"/>
+      <c r="K18" s="144"/>
+      <c r="L18" s="145"/>
+      <c r="M18" s="145"/>
+      <c r="N18" s="146"/>
       <c r="O18" s="70"/>
       <c r="P18" s="89"/>
       <c r="Q18" s="89"/>
@@ -4795,22 +5274,22 @@
       <c r="T18" s="57"/>
     </row>
     <row r="19" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="153" t="s">
+      <c r="A19" s="167" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="154"/>
-      <c r="C19" s="155"/>
-      <c r="D19" s="156"/>
-      <c r="E19" s="156"/>
-      <c r="F19" s="157"/>
+      <c r="B19" s="168"/>
+      <c r="C19" s="169"/>
+      <c r="D19" s="170"/>
+      <c r="E19" s="170"/>
+      <c r="F19" s="171"/>
       <c r="G19" s="91"/>
       <c r="H19" s="92"/>
       <c r="I19" s="93"/>
       <c r="J19" s="94"/>
-      <c r="K19" s="158"/>
-      <c r="L19" s="159"/>
-      <c r="M19" s="159"/>
-      <c r="N19" s="160"/>
+      <c r="K19" s="172"/>
+      <c r="L19" s="173"/>
+      <c r="M19" s="173"/>
+      <c r="N19" s="174"/>
       <c r="O19" s="71"/>
       <c r="P19" s="95"/>
       <c r="Q19" s="95"/>
@@ -4819,22 +5298,22 @@
       <c r="T19" s="57"/>
     </row>
     <row r="20" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="131" t="s">
+      <c r="A20" s="147" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="132"/>
-      <c r="C20" s="133"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="134"/>
-      <c r="F20" s="135"/>
+      <c r="B20" s="148"/>
+      <c r="C20" s="149"/>
+      <c r="D20" s="150"/>
+      <c r="E20" s="150"/>
+      <c r="F20" s="151"/>
       <c r="G20" s="97"/>
       <c r="H20" s="98"/>
       <c r="I20" s="99"/>
       <c r="J20" s="97"/>
-      <c r="K20" s="136"/>
-      <c r="L20" s="137"/>
-      <c r="M20" s="137"/>
-      <c r="N20" s="138"/>
+      <c r="K20" s="152"/>
+      <c r="L20" s="153"/>
+      <c r="M20" s="153"/>
+      <c r="N20" s="154"/>
       <c r="O20" s="72"/>
       <c r="P20" s="100"/>
       <c r="Q20" s="100"/>
@@ -4844,13 +5323,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="K18:N18"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="K20:N20"/>
@@ -4866,6 +5338,13 @@
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="K17:N17"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="K18:N18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q3" location="'Objeto Dominio N'!A16" display="'Objeto Dominio N'!A16" xr:uid="{48F15180-B8A0-4BDB-9A1D-A23E44A10E26}"/>
@@ -4891,7 +5370,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4921,70 +5400,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="O1" s="120"/>
-      <c r="P1" s="120"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="121" t="str">
+      <c r="B2" s="106" t="str">
         <f>'Listado Objetos de Dominio'!$A$4</f>
         <v>Tarea</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
-      <c r="P2" s="121"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="122" t="str">
+      <c r="B3" s="107" t="str">
         <f>'Listado Objetos de Dominio'!$B$4</f>
         <v>Este objeto de dominio contiene la información de una tarea que esta dentro de una listaTarea</v>
       </c>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="122"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="122"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="107"/>
+      <c r="O3" s="107"/>
+      <c r="P3" s="107"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -5052,7 +5531,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
         <v>37</v>
       </c>
@@ -5098,7 +5577,7 @@
       <c r="S5" s="28"/>
       <c r="T5" s="31"/>
     </row>
-    <row r="6" spans="1:20" ht="51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
@@ -5384,44 +5863,44 @@
     </row>
     <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="126" t="s">
+      <c r="A14" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="127"/>
-      <c r="C14" s="127" t="s">
+      <c r="B14" s="112"/>
+      <c r="C14" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="127"/>
-      <c r="E14" s="127"/>
-      <c r="F14" s="127"/>
-      <c r="G14" s="127" t="s">
+      <c r="D14" s="112"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="127"/>
-      <c r="I14" s="127"/>
-      <c r="J14" s="127" t="s">
+      <c r="H14" s="112"/>
+      <c r="I14" s="112"/>
+      <c r="J14" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="127"/>
-      <c r="L14" s="127"/>
-      <c r="M14" s="127"/>
-      <c r="N14" s="127"/>
-      <c r="O14" s="127" t="s">
+      <c r="K14" s="112"/>
+      <c r="L14" s="112"/>
+      <c r="M14" s="112"/>
+      <c r="N14" s="112"/>
+      <c r="O14" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="127"/>
-      <c r="Q14" s="127" t="s">
+      <c r="P14" s="112"/>
+      <c r="Q14" s="112" t="s">
         <v>27</v>
       </c>
       <c r="R14" s="130"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="128"/>
-      <c r="B15" s="129"/>
-      <c r="C15" s="129"/>
-      <c r="D15" s="129"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="129"/>
+      <c r="A15" s="113"/>
+      <c r="B15" s="114"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="114"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="114"/>
       <c r="G15" s="19" t="s">
         <v>28</v>
       </c>
@@ -5434,12 +5913,12 @@
       <c r="J15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="129" t="s">
+      <c r="K15" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="L15" s="129"/>
-      <c r="M15" s="129"/>
-      <c r="N15" s="129"/>
+      <c r="L15" s="114"/>
+      <c r="M15" s="114"/>
+      <c r="N15" s="114"/>
       <c r="O15" s="19" t="s">
         <v>30</v>
       </c>
@@ -5454,88 +5933,88 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="113" t="s">
+      <c r="A16" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="114"/>
-      <c r="C16" s="115"/>
-      <c r="D16" s="115"/>
-      <c r="E16" s="115"/>
-      <c r="F16" s="115"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
       <c r="G16" s="20"/>
       <c r="H16" s="21"/>
       <c r="I16" s="22"/>
       <c r="J16" s="21"/>
-      <c r="K16" s="115"/>
-      <c r="L16" s="115"/>
-      <c r="M16" s="115"/>
-      <c r="N16" s="115"/>
+      <c r="K16" s="117"/>
+      <c r="L16" s="117"/>
+      <c r="M16" s="117"/>
+      <c r="N16" s="117"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="20"/>
       <c r="R16" s="26"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="116" t="s">
+      <c r="A17" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
       <c r="G17" s="46"/>
       <c r="H17" s="44"/>
       <c r="I17" s="45"/>
       <c r="J17" s="39"/>
-      <c r="K17" s="119"/>
-      <c r="L17" s="119"/>
-      <c r="M17" s="119"/>
-      <c r="N17" s="119"/>
+      <c r="K17" s="121"/>
+      <c r="L17" s="121"/>
+      <c r="M17" s="121"/>
+      <c r="N17" s="121"/>
       <c r="O17" s="23"/>
       <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
       <c r="R17" s="27"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="105" t="s">
+      <c r="A18" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="106"/>
-      <c r="C18" s="107"/>
-      <c r="D18" s="107"/>
-      <c r="E18" s="107"/>
-      <c r="F18" s="107"/>
+      <c r="B18" s="123"/>
+      <c r="C18" s="124"/>
+      <c r="D18" s="124"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="124"/>
       <c r="G18" s="42"/>
       <c r="H18" s="40"/>
       <c r="I18" s="41"/>
       <c r="J18" s="43"/>
-      <c r="K18" s="108"/>
-      <c r="L18" s="108"/>
-      <c r="M18" s="108"/>
-      <c r="N18" s="108"/>
+      <c r="K18" s="125"/>
+      <c r="L18" s="125"/>
+      <c r="M18" s="125"/>
+      <c r="N18" s="125"/>
       <c r="O18" s="28"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="29"/>
       <c r="R18" s="30"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="109" t="s">
+      <c r="A19" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="110"/>
-      <c r="C19" s="111"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
+      <c r="B19" s="127"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="128"/>
+      <c r="E19" s="128"/>
+      <c r="F19" s="128"/>
       <c r="G19" s="48"/>
       <c r="H19" s="49"/>
       <c r="I19" s="47"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="112"/>
-      <c r="L19" s="112"/>
-      <c r="M19" s="112"/>
-      <c r="N19" s="112"/>
+      <c r="K19" s="129"/>
+      <c r="L19" s="129"/>
+      <c r="M19" s="129"/>
+      <c r="N19" s="129"/>
       <c r="O19" s="31"/>
       <c r="P19" s="32"/>
       <c r="Q19" s="32"/>
@@ -5543,17 +6022,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="K16:N16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="K17:N17"/>
@@ -5565,6 +6033,17 @@
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="J14:N14"/>
     <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="K19:N19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{3D0D9E13-D1D9-441A-A3A1-ED77A0A4DA4F}"/>
@@ -5620,70 +6099,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="O1" s="120"/>
-      <c r="P1" s="120"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="121" t="str">
+      <c r="B2" s="106" t="str">
         <f>'Listado Objetos de Dominio'!$A$5</f>
         <v>Estado</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
-      <c r="P2" s="121"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="122" t="str">
+      <c r="B3" s="107" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v>Este objeto de dominio contiene el estado de realización en el que puede estar una lista de tareas o una tarea</v>
       </c>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="122"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="122"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="107"/>
+      <c r="O3" s="107"/>
+      <c r="P3" s="107"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -5845,44 +6324,44 @@
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="126" t="s">
+      <c r="A8" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="127"/>
-      <c r="C8" s="127" t="s">
+      <c r="B8" s="112"/>
+      <c r="C8" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="127"/>
-      <c r="E8" s="127"/>
-      <c r="F8" s="127"/>
-      <c r="G8" s="127" t="s">
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
+      <c r="G8" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="127"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="127" t="s">
+      <c r="H8" s="112"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="127"/>
-      <c r="L8" s="127"/>
-      <c r="M8" s="127"/>
-      <c r="N8" s="127"/>
-      <c r="O8" s="127" t="s">
+      <c r="K8" s="112"/>
+      <c r="L8" s="112"/>
+      <c r="M8" s="112"/>
+      <c r="N8" s="112"/>
+      <c r="O8" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="P8" s="127"/>
-      <c r="Q8" s="127" t="s">
+      <c r="P8" s="112"/>
+      <c r="Q8" s="112" t="s">
         <v>27</v>
       </c>
       <c r="R8" s="130"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="128"/>
-      <c r="B9" s="129"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="129"/>
-      <c r="E9" s="129"/>
-      <c r="F9" s="129"/>
+      <c r="A9" s="113"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
       <c r="G9" s="19" t="s">
         <v>28</v>
       </c>
@@ -5895,12 +6374,12 @@
       <c r="J9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="129" t="s">
+      <c r="K9" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="129"/>
-      <c r="M9" s="129"/>
-      <c r="N9" s="129"/>
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="N9" s="114"/>
       <c r="O9" s="19" t="s">
         <v>30</v>
       </c>
@@ -5915,88 +6394,88 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="114"/>
-      <c r="C10" s="115"/>
-      <c r="D10" s="115"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="115"/>
+      <c r="B10" s="116"/>
+      <c r="C10" s="117"/>
+      <c r="D10" s="117"/>
+      <c r="E10" s="117"/>
+      <c r="F10" s="117"/>
       <c r="G10" s="20"/>
       <c r="H10" s="21"/>
       <c r="I10" s="22"/>
       <c r="J10" s="21"/>
-      <c r="K10" s="115"/>
-      <c r="L10" s="115"/>
-      <c r="M10" s="115"/>
-      <c r="N10" s="115"/>
+      <c r="K10" s="117"/>
+      <c r="L10" s="117"/>
+      <c r="M10" s="117"/>
+      <c r="N10" s="117"/>
       <c r="O10" s="20"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="26"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="117"/>
-      <c r="C11" s="118"/>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="120"/>
       <c r="G11" s="46"/>
       <c r="H11" s="44"/>
       <c r="I11" s="45"/>
       <c r="J11" s="39"/>
-      <c r="K11" s="119"/>
-      <c r="L11" s="119"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="119"/>
+      <c r="K11" s="121"/>
+      <c r="L11" s="121"/>
+      <c r="M11" s="121"/>
+      <c r="N11" s="121"/>
       <c r="O11" s="23"/>
       <c r="P11" s="24"/>
       <c r="Q11" s="24"/>
       <c r="R11" s="27"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="105" t="s">
+      <c r="A12" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="106"/>
-      <c r="C12" s="107"/>
-      <c r="D12" s="107"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
+      <c r="B12" s="123"/>
+      <c r="C12" s="124"/>
+      <c r="D12" s="124"/>
+      <c r="E12" s="124"/>
+      <c r="F12" s="124"/>
       <c r="G12" s="42"/>
       <c r="H12" s="40"/>
       <c r="I12" s="41"/>
       <c r="J12" s="43"/>
-      <c r="K12" s="108"/>
-      <c r="L12" s="108"/>
-      <c r="M12" s="108"/>
-      <c r="N12" s="108"/>
+      <c r="K12" s="125"/>
+      <c r="L12" s="125"/>
+      <c r="M12" s="125"/>
+      <c r="N12" s="125"/>
       <c r="O12" s="28"/>
       <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
       <c r="R12" s="30"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="110"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
+      <c r="B13" s="127"/>
+      <c r="C13" s="128"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="128"/>
+      <c r="F13" s="128"/>
       <c r="G13" s="48"/>
       <c r="H13" s="49"/>
       <c r="I13" s="47"/>
       <c r="J13" s="48"/>
-      <c r="K13" s="112"/>
-      <c r="L13" s="112"/>
-      <c r="M13" s="112"/>
-      <c r="N13" s="112"/>
+      <c r="K13" s="129"/>
+      <c r="L13" s="129"/>
+      <c r="M13" s="129"/>
+      <c r="N13" s="129"/>
       <c r="O13" s="31"/>
       <c r="P13" s="32"/>
       <c r="Q13" s="32"/>
@@ -6004,17 +6483,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="K10:N10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="K11:N11"/>
@@ -6026,6 +6494,17 @@
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="J8:N8"/>
     <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="K13:N13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{732AA0A1-838F-4143-B4CB-8A43F6533B73}"/>
@@ -6046,6 +6525,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001D0DE5568C0AE848B2F225150E15E78E" ma:contentTypeVersion="3" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="643d399a24376eab49db33c80db032ac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="915fd109-ae29-4648-8de1-7f064f1d0fe5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2a54904d818499acdea7742e4a0622bc" ns2:_="">
     <xsd:import namespace="915fd109-ae29-4648-8de1-7f064f1d0fe5"/>
@@ -6183,15 +6671,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6199,6 +6678,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C779E5F7-74AC-4CCB-8FB1-CBA1DF721FBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6212,14 +6699,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Agregar rcr proyecto en modelo enriquecido proyectos
</commit_message>
<xml_diff>
--- a/ModelosEnriquecidos/Modelo enriquecido - Proyecto.xlsx
+++ b/ModelosEnriquecidos/Modelo enriquecido - Proyecto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Información\Downloads\DOO-working-group\ModelosEnriquecidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B86BBD-8FBB-4B3E-900E-2557CFB6230B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B5F608-F204-4F37-8F08-11DB5940D480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" firstSheet="2" activeTab="2" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de dominio anémico" sheetId="61" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="ObjetoDominio Tarea" sheetId="69" r:id="rId7"/>
     <sheet name="ObjetoDominio Estado" sheetId="70" r:id="rId8"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Listado Objetos de Dominio'!$A$1:$B$7</definedName>
   </definedNames>
@@ -46,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="200">
   <si>
     <t>Nombre</t>
   </si>
@@ -504,13 +507,148 @@
     <t>Requerido</t>
   </si>
   <si>
-    <t>RequeridoOpcional</t>
-  </si>
-  <si>
-    <t>RequeridaOpcional</t>
-  </si>
-  <si>
-    <t>No requerido</t>
+    <t>ModificarNombreDescripcion</t>
+  </si>
+  <si>
+    <t>Permite modificar el nombre y/o la descripción de un proyecto existente</t>
+  </si>
+  <si>
+    <t>Contiene los datos que se requieren modificar</t>
+  </si>
+  <si>
+    <t>Sólo un miebro del equipo asociado al proyecto puede modificarlo</t>
+  </si>
+  <si>
+    <t>El valor del atributo que se desea modificar no debe ser igual al valor del atributo que esta previamente</t>
+  </si>
+  <si>
+    <t>Debe existir el identificador del proyecto el cual va a ser modificado</t>
+  </si>
+  <si>
+    <t>El usuario que quiere modificar el proyecto no pertenece al equipo del proyecto</t>
+  </si>
+  <si>
+    <t>El valor ingresado a modificar es el mismo valor que se encuentra actualmente en el atributo</t>
+  </si>
+  <si>
+    <t>Abortar y notificar al usuario que solicite acceso al proyecto</t>
+  </si>
+  <si>
+    <t>Abortar y notificar que el valor ingresado a cambiar ya estaba previamente asginado</t>
+  </si>
+  <si>
+    <t>El identificador del proyecto a modificar no existe y por tanto no existe tal proyecto</t>
+  </si>
+  <si>
+    <t>Abortar y notificar que el identificador asociado al proyecto no existe</t>
+  </si>
+  <si>
+    <t>ModificarFechaFinalizacion</t>
+  </si>
+  <si>
+    <t>Permite modificar la fecha de finalización asginada a un proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contiene los datos que se requieren modificar </t>
+  </si>
+  <si>
+    <t>ModificarParticipantes</t>
+  </si>
+  <si>
+    <t>Permite modificar el atributo que rastrea el numero de participantes que tiene un proyecto</t>
+  </si>
+  <si>
+    <t>El numero de integrantes no puede ser cero</t>
+  </si>
+  <si>
+    <t>El numero de integrantes es 0 lo cual significaria que no hay ningun usuario en el equipo asociado al proyecto</t>
+  </si>
+  <si>
+    <t>Advertir que la modificación en los participantes del equipo causara que el proyecto sea eliminado</t>
+  </si>
+  <si>
+    <t>Consultar</t>
+  </si>
+  <si>
+    <t>Eliminar</t>
+  </si>
+  <si>
+    <t>Permite consultar los proyectos existentes que cumplan con los criterios de busqueda enviados</t>
+  </si>
+  <si>
+    <t>Proyecto[]</t>
+  </si>
+  <si>
+    <t>Contiene un conjunto de proyectos que cumplen con los criterios de filtrado</t>
+  </si>
+  <si>
+    <t>Contiene los datos filtrados que se requieren consultar</t>
+  </si>
+  <si>
+    <t>Permite eliminar definitivamente un proyecto</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>Alfanumerico</t>
+  </si>
+  <si>
+    <t>Se refiere el identificador del proyecto que se va a eliminar</t>
+  </si>
+  <si>
+    <t>Debe existir el identificador del proyecto el cual va a ser eliminado</t>
+  </si>
+  <si>
+    <t>Solo el dueño del equipo asginado al proyecto puede eliminarlo</t>
+  </si>
+  <si>
+    <t>El identificador del proyecto a eliminar no existe y por tanto no existe tal proyecto</t>
+  </si>
+  <si>
+    <t>Abortar y notificar que no existe un proyecto vinculado a el identificador enviado</t>
+  </si>
+  <si>
+    <t>Solo el participante con el rol de dueño puede eliminar el proyecto</t>
+  </si>
+  <si>
+    <t>Abortar y notificar que el unico rol que tiene el permiso de eliminar un proyecto es el dueño del equipo y  del proyecto</t>
+  </si>
+  <si>
+    <t>Requerido/NoModificable</t>
+  </si>
+  <si>
+    <t>Requerido/Opcional</t>
+  </si>
+  <si>
+    <t>NoRequerido</t>
+  </si>
+  <si>
+    <t>Requerido/Modificable</t>
+  </si>
+  <si>
+    <t>Filtro/NoMostrar{Usuario}/Mostrar{Aplicación}</t>
+  </si>
+  <si>
+    <t>Filtro/Mostrar{Usuario,Sistema}-Orden1{Defecto:Desc}</t>
+  </si>
+  <si>
+    <t>Filtro/Mostrar{Usuario,Sistema}-Orden2{Defecto:Desc}</t>
+  </si>
+  <si>
+    <t>Filtro/Mostrar{Usuario,Sistema}-Orden3{Defecto:Desc}</t>
+  </si>
+  <si>
+    <t>Filtro/Mostrar{Usuario,Sistema}-Orden4{Defecto:Desc}</t>
+  </si>
+  <si>
+    <t>Filtro/Mostrar{Usuario,Sistema}-Orden7{Defecto:Desc}</t>
+  </si>
+  <si>
+    <t>Filtro/NoMostrar{Usuario}-Orden5{Defecto:Desc}-{Propiedad: CorreoElectronico, cargo}</t>
+  </si>
+  <si>
+    <t>Filtro/Mostrar{Usuario,Sistema}-Orden6{Defecto:Desc}-{Propiedad: Nombre}</t>
   </si>
 </sst>
 </file>
@@ -604,7 +742,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -713,6 +851,18 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="39">
     <border>
@@ -1190,7 +1340,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="301">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1502,6 +1652,30 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1532,54 +1706,144 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="38" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1736,118 +2000,244 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="38" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="33" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="30" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="38" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="38" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="35" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1939,6 +2329,36 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Flujo de eventos anémico"/>
+      <sheetName val="Listado Objetos de Dominio"/>
+      <sheetName val="Participante"/>
+      <sheetName val="Proyecto"/>
+      <sheetName val="ListaTareas"/>
+      <sheetName val="Tarea"/>
+      <sheetName val="Estado"/>
+      <sheetName val="MetricaProyecto"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2241,7 +2661,7 @@
   <dimension ref="A1:V50"/>
   <sheetViews>
     <sheetView topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W63" sqref="W63"/>
+      <selection activeCell="AA49" sqref="AA49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,93 +2820,100 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD37FF8E-62F4-4178-9B49-EEA97FFC0EF4}">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="16" max="16" width="92.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" hidden="1" customWidth="1"/>
+    <col min="11" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="92.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="42.140625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="60.7109375" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="27.5703125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="25.28515625" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="80.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="106" t="str">
+      <c r="B2" s="114" t="str">
         <f>'Listado Objetos de Dominio'!$A$6</f>
         <v>Proyecto</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
-      <c r="N2" s="106"/>
-      <c r="O2" s="106"/>
-      <c r="P2" s="106"/>
-    </row>
-    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="114"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="114"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="107" t="str">
+      <c r="B3" s="115" t="str">
         <f>'Listado Objetos de Dominio'!$B$6</f>
         <v>Este objeto de dominio es la razon principal de la aplicaicion y me describe un esfuerzo general para lograr un resultado</v>
       </c>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="115"/>
+      <c r="O3" s="115"/>
+      <c r="P3" s="115"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -2535,24 +2962,32 @@
       <c r="P4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="Q4" s="220" t="str">
+      <c r="Q4" s="106" t="str">
         <f>A20</f>
         <v>Crear</v>
       </c>
-      <c r="R4" s="35" t="str">
-        <f>A20</f>
-        <v>Crear</v>
-      </c>
-      <c r="S4" s="36" t="str">
+      <c r="R4" s="267" t="str">
         <f>A24</f>
-        <v>Reponsabilidad 2</v>
-      </c>
-      <c r="T4" s="2" t="str">
-        <f>A25</f>
-        <v>Reponsabilidad 3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="127.5" x14ac:dyDescent="0.25">
+        <v>ModificarNombreDescripcion</v>
+      </c>
+      <c r="S4" s="291" t="str">
+        <f>A27</f>
+        <v>ModificarFechaFinalizacion</v>
+      </c>
+      <c r="T4" s="292" t="str">
+        <f>A31</f>
+        <v>ModificarParticipantes</v>
+      </c>
+      <c r="U4" s="299" t="str">
+        <f>A34</f>
+        <v>Consultar</v>
+      </c>
+      <c r="V4" s="300" t="str">
+        <f>A35</f>
+        <v>Eliminar</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
         <v>59</v>
       </c>
@@ -2596,11 +3031,23 @@
       <c r="Q5" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="R5" s="23"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="31"/>
-    </row>
-    <row r="6" spans="1:20" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="R5" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="S5" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="T5" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="U5" s="273" t="s">
+        <v>192</v>
+      </c>
+      <c r="V5" s="274" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
@@ -2644,11 +3091,23 @@
       <c r="Q6" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="R6" s="23"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="31"/>
-    </row>
-    <row r="7" spans="1:20" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="R6" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="S6" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="T6" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="U6" s="273" t="s">
+        <v>193</v>
+      </c>
+      <c r="V6" s="274" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>1</v>
       </c>
@@ -2690,13 +3149,25 @@
         <v>129</v>
       </c>
       <c r="Q7" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="R7" s="23"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="31"/>
-    </row>
-    <row r="8" spans="1:20" ht="51" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="R7" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="S7" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="T7" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="U7" s="273" t="s">
+        <v>194</v>
+      </c>
+      <c r="V7" s="274" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>47</v>
       </c>
@@ -2732,11 +3203,23 @@
       <c r="Q8" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="R8" s="23"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="31"/>
-    </row>
-    <row r="9" spans="1:20" ht="51" x14ac:dyDescent="0.25">
+      <c r="R8" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="S8" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="T8" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="U8" s="273" t="s">
+        <v>195</v>
+      </c>
+      <c r="V8" s="274" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>48</v>
       </c>
@@ -2770,13 +3253,25 @@
         <v>131</v>
       </c>
       <c r="Q9" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="R9" s="23"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="31"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="R9" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="S9" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="T9" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="U9" s="273" t="s">
+        <v>196</v>
+      </c>
+      <c r="V9" s="274" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>134</v>
       </c>
@@ -2800,11 +3295,23 @@
       <c r="Q10" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="R10" s="23"/>
-      <c r="S10" s="28"/>
-      <c r="T10" s="31"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R10" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="S10" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="T10" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="U10" s="273" t="s">
+        <v>198</v>
+      </c>
+      <c r="V10" s="274" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>133</v>
       </c>
@@ -2826,13 +3333,25 @@
       <c r="O11" s="5"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="R11" s="23"/>
-      <c r="S11" s="28"/>
-      <c r="T11" s="31"/>
-    </row>
-    <row r="12" spans="1:20" ht="76.5" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="R11" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="S11" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="T11" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="U11" s="273" t="s">
+        <v>199</v>
+      </c>
+      <c r="V11" s="274" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>90</v>
       </c>
@@ -2880,11 +3399,23 @@
       <c r="Q12" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="R12" s="23"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="31"/>
-    </row>
-    <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R12" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="S12" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="T12" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="U12" s="273" t="s">
+        <v>197</v>
+      </c>
+      <c r="V12" s="274" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2902,12 +3433,12 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="108" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="109"/>
-      <c r="C14" s="110"/>
+      <c r="B14" s="117"/>
+      <c r="C14" s="118"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2922,7 +3453,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>21</v>
       </c>
@@ -2946,7 +3477,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="103"/>
@@ -2983,44 +3514,44 @@
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="111" t="s">
+      <c r="A18" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="112"/>
-      <c r="C18" s="112" t="s">
+      <c r="B18" s="120"/>
+      <c r="C18" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="112" t="s">
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
+      <c r="G18" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="112"/>
-      <c r="I18" s="112"/>
-      <c r="J18" s="112" t="s">
+      <c r="H18" s="120"/>
+      <c r="I18" s="120"/>
+      <c r="J18" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="K18" s="112"/>
-      <c r="L18" s="112"/>
-      <c r="M18" s="112"/>
-      <c r="N18" s="112"/>
-      <c r="O18" s="112" t="s">
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="120"/>
+      <c r="N18" s="120"/>
+      <c r="O18" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="P18" s="112"/>
-      <c r="Q18" s="112" t="s">
+      <c r="P18" s="120"/>
+      <c r="Q18" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="R18" s="130"/>
+      <c r="R18" s="135"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="113"/>
-      <c r="B19" s="114"/>
-      <c r="C19" s="114"/>
-      <c r="D19" s="114"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="114"/>
+      <c r="A19" s="121"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="122"/>
       <c r="G19" s="19" t="s">
         <v>28</v>
       </c>
@@ -3033,12 +3564,12 @@
       <c r="J19" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K19" s="114" t="s">
+      <c r="K19" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="L19" s="114"/>
-      <c r="M19" s="114"/>
-      <c r="N19" s="114"/>
+      <c r="L19" s="122"/>
+      <c r="M19" s="122"/>
+      <c r="N19" s="122"/>
       <c r="O19" s="19" t="s">
         <v>30</v>
       </c>
@@ -3053,30 +3584,30 @@
       </c>
     </row>
     <row r="20" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="196" t="s">
+      <c r="A20" s="136" t="s">
         <v>136</v>
       </c>
-      <c r="B20" s="197"/>
-      <c r="C20" s="202" t="s">
+      <c r="B20" s="137"/>
+      <c r="C20" s="142" t="s">
         <v>137</v>
       </c>
-      <c r="D20" s="203"/>
-      <c r="E20" s="203"/>
-      <c r="F20" s="204"/>
-      <c r="G20" s="211" t="s">
+      <c r="D20" s="143"/>
+      <c r="E20" s="143"/>
+      <c r="F20" s="144"/>
+      <c r="G20" s="151" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="214" t="s">
+      <c r="H20" s="154" t="s">
         <v>126</v>
       </c>
-      <c r="I20" s="217" t="s">
+      <c r="I20" s="157" t="s">
         <v>138</v>
       </c>
-      <c r="J20" s="214"/>
-      <c r="K20" s="202"/>
-      <c r="L20" s="203"/>
-      <c r="M20" s="203"/>
-      <c r="N20" s="204"/>
+      <c r="J20" s="154"/>
+      <c r="K20" s="142"/>
+      <c r="L20" s="143"/>
+      <c r="M20" s="143"/>
+      <c r="N20" s="144"/>
       <c r="O20" s="20">
         <v>1</v>
       </c>
@@ -3086,25 +3617,25 @@
       <c r="Q20" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="R20" s="195" t="s">
+      <c r="R20" s="105" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="198"/>
-      <c r="B21" s="199"/>
-      <c r="C21" s="205"/>
-      <c r="D21" s="206"/>
-      <c r="E21" s="206"/>
-      <c r="F21" s="207"/>
-      <c r="G21" s="212"/>
-      <c r="H21" s="215"/>
-      <c r="I21" s="218"/>
-      <c r="J21" s="215"/>
-      <c r="K21" s="205"/>
-      <c r="L21" s="206"/>
-      <c r="M21" s="206"/>
-      <c r="N21" s="207"/>
+      <c r="A21" s="138"/>
+      <c r="B21" s="139"/>
+      <c r="C21" s="145"/>
+      <c r="D21" s="146"/>
+      <c r="E21" s="146"/>
+      <c r="F21" s="147"/>
+      <c r="G21" s="152"/>
+      <c r="H21" s="155"/>
+      <c r="I21" s="158"/>
+      <c r="J21" s="155"/>
+      <c r="K21" s="145"/>
+      <c r="L21" s="146"/>
+      <c r="M21" s="146"/>
+      <c r="N21" s="147"/>
       <c r="O21" s="20">
         <v>2</v>
       </c>
@@ -3119,20 +3650,20 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="198"/>
-      <c r="B22" s="199"/>
-      <c r="C22" s="205"/>
-      <c r="D22" s="206"/>
-      <c r="E22" s="206"/>
-      <c r="F22" s="207"/>
-      <c r="G22" s="212"/>
-      <c r="H22" s="215"/>
-      <c r="I22" s="218"/>
-      <c r="J22" s="215"/>
-      <c r="K22" s="205"/>
-      <c r="L22" s="206"/>
-      <c r="M22" s="206"/>
-      <c r="N22" s="207"/>
+      <c r="A22" s="138"/>
+      <c r="B22" s="139"/>
+      <c r="C22" s="145"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="147"/>
+      <c r="G22" s="152"/>
+      <c r="H22" s="155"/>
+      <c r="I22" s="158"/>
+      <c r="J22" s="155"/>
+      <c r="K22" s="145"/>
+      <c r="L22" s="146"/>
+      <c r="M22" s="146"/>
+      <c r="N22" s="147"/>
       <c r="O22" s="20">
         <v>3</v>
       </c>
@@ -3147,20 +3678,20 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="200"/>
-      <c r="B23" s="201"/>
-      <c r="C23" s="208"/>
-      <c r="D23" s="209"/>
-      <c r="E23" s="209"/>
-      <c r="F23" s="210"/>
-      <c r="G23" s="213"/>
-      <c r="H23" s="216"/>
-      <c r="I23" s="219"/>
-      <c r="J23" s="216"/>
-      <c r="K23" s="208"/>
-      <c r="L23" s="209"/>
-      <c r="M23" s="209"/>
-      <c r="N23" s="210"/>
+      <c r="A23" s="140"/>
+      <c r="B23" s="141"/>
+      <c r="C23" s="148"/>
+      <c r="D23" s="149"/>
+      <c r="E23" s="149"/>
+      <c r="F23" s="150"/>
+      <c r="G23" s="153"/>
+      <c r="H23" s="156"/>
+      <c r="I23" s="159"/>
+      <c r="J23" s="156"/>
+      <c r="K23" s="148"/>
+      <c r="L23" s="149"/>
+      <c r="M23" s="149"/>
+      <c r="N23" s="150"/>
       <c r="O23" s="20">
         <v>4</v>
       </c>
@@ -3174,74 +3705,437 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="118" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="119"/>
-      <c r="C24" s="120"/>
-      <c r="D24" s="120"/>
-      <c r="E24" s="120"/>
-      <c r="F24" s="120"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="121"/>
-      <c r="L24" s="121"/>
-      <c r="M24" s="121"/>
-      <c r="N24" s="121"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="122" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="123"/>
-      <c r="C25" s="124"/>
-      <c r="D25" s="124"/>
-      <c r="E25" s="124"/>
-      <c r="F25" s="124"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="125"/>
-      <c r="L25" s="125"/>
-      <c r="M25" s="125"/>
-      <c r="N25" s="125"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="29"/>
-      <c r="Q25" s="29"/>
-      <c r="R25" s="29"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="126" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="127"/>
-      <c r="C26" s="128"/>
-      <c r="D26" s="128"/>
-      <c r="E26" s="128"/>
-      <c r="F26" s="128"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="129"/>
-      <c r="L26" s="129"/>
-      <c r="M26" s="129"/>
-      <c r="N26" s="129"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="32"/>
-      <c r="Q26" s="32"/>
-      <c r="R26" s="32"/>
+    <row r="24" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="221" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" s="222"/>
+      <c r="C24" s="230" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="231"/>
+      <c r="E24" s="231"/>
+      <c r="F24" s="232"/>
+      <c r="G24" s="227" t="s">
+        <v>126</v>
+      </c>
+      <c r="H24" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="I24" s="242" t="s">
+        <v>154</v>
+      </c>
+      <c r="J24" s="227"/>
+      <c r="K24" s="230"/>
+      <c r="L24" s="231"/>
+      <c r="M24" s="231"/>
+      <c r="N24" s="232"/>
+      <c r="O24" s="23">
+        <v>5</v>
+      </c>
+      <c r="P24" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q24" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="R24" s="24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="223"/>
+      <c r="B25" s="224"/>
+      <c r="C25" s="233"/>
+      <c r="D25" s="234"/>
+      <c r="E25" s="234"/>
+      <c r="F25" s="235"/>
+      <c r="G25" s="228"/>
+      <c r="H25" s="240"/>
+      <c r="I25" s="243"/>
+      <c r="J25" s="228"/>
+      <c r="K25" s="233"/>
+      <c r="L25" s="234"/>
+      <c r="M25" s="234"/>
+      <c r="N25" s="235"/>
+      <c r="O25" s="23">
+        <v>6</v>
+      </c>
+      <c r="P25" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q25" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="R25" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="225"/>
+      <c r="B26" s="226"/>
+      <c r="C26" s="236"/>
+      <c r="D26" s="237"/>
+      <c r="E26" s="237"/>
+      <c r="F26" s="238"/>
+      <c r="G26" s="229"/>
+      <c r="H26" s="241"/>
+      <c r="I26" s="244"/>
+      <c r="J26" s="229"/>
+      <c r="K26" s="236"/>
+      <c r="L26" s="237"/>
+      <c r="M26" s="237"/>
+      <c r="N26" s="238"/>
+      <c r="O26" s="23">
+        <v>7</v>
+      </c>
+      <c r="P26" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q26" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="R26" s="24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="257" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27" s="258"/>
+      <c r="C27" s="248" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" s="249"/>
+      <c r="E27" s="249"/>
+      <c r="F27" s="250"/>
+      <c r="G27" s="261" t="s">
+        <v>126</v>
+      </c>
+      <c r="H27" s="264" t="s">
+        <v>126</v>
+      </c>
+      <c r="I27" s="268" t="s">
+        <v>166</v>
+      </c>
+      <c r="J27" s="261"/>
+      <c r="K27" s="248"/>
+      <c r="L27" s="249"/>
+      <c r="M27" s="249"/>
+      <c r="N27" s="250"/>
+      <c r="O27" s="28">
+        <v>4</v>
+      </c>
+      <c r="P27" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q27" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="R27" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="259"/>
+      <c r="B28" s="260"/>
+      <c r="C28" s="251"/>
+      <c r="D28" s="252"/>
+      <c r="E28" s="252"/>
+      <c r="F28" s="253"/>
+      <c r="G28" s="262"/>
+      <c r="H28" s="265"/>
+      <c r="I28" s="269"/>
+      <c r="J28" s="262"/>
+      <c r="K28" s="251"/>
+      <c r="L28" s="252"/>
+      <c r="M28" s="252"/>
+      <c r="N28" s="253"/>
+      <c r="O28" s="28">
+        <v>5</v>
+      </c>
+      <c r="P28" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q28" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="R28" s="29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="259"/>
+      <c r="B29" s="260"/>
+      <c r="C29" s="251"/>
+      <c r="D29" s="252"/>
+      <c r="E29" s="252"/>
+      <c r="F29" s="253"/>
+      <c r="G29" s="262"/>
+      <c r="H29" s="265"/>
+      <c r="I29" s="269"/>
+      <c r="J29" s="262"/>
+      <c r="K29" s="251"/>
+      <c r="L29" s="252"/>
+      <c r="M29" s="252"/>
+      <c r="N29" s="253"/>
+      <c r="O29" s="28">
+        <v>6</v>
+      </c>
+      <c r="P29" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q29" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="R29" s="29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="245"/>
+      <c r="B30" s="246"/>
+      <c r="C30" s="254"/>
+      <c r="D30" s="255"/>
+      <c r="E30" s="255"/>
+      <c r="F30" s="256"/>
+      <c r="G30" s="263"/>
+      <c r="H30" s="266"/>
+      <c r="I30" s="270"/>
+      <c r="J30" s="263"/>
+      <c r="K30" s="254"/>
+      <c r="L30" s="255"/>
+      <c r="M30" s="255"/>
+      <c r="N30" s="256"/>
+      <c r="O30" s="28">
+        <v>7</v>
+      </c>
+      <c r="P30" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q30" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="R30" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="247" t="s">
+        <v>167</v>
+      </c>
+      <c r="B31" s="247"/>
+      <c r="C31" s="134" t="s">
+        <v>168</v>
+      </c>
+      <c r="D31" s="134"/>
+      <c r="E31" s="134"/>
+      <c r="F31" s="134"/>
+      <c r="G31" s="271" t="s">
+        <v>126</v>
+      </c>
+      <c r="H31" s="272" t="s">
+        <v>126</v>
+      </c>
+      <c r="I31" s="134" t="s">
+        <v>166</v>
+      </c>
+      <c r="J31" s="271"/>
+      <c r="K31" s="134"/>
+      <c r="L31" s="134"/>
+      <c r="M31" s="134"/>
+      <c r="N31" s="134"/>
+      <c r="O31" s="31">
+        <v>6</v>
+      </c>
+      <c r="P31" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q31" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="R31" s="32" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="247"/>
+      <c r="B32" s="247"/>
+      <c r="C32" s="134"/>
+      <c r="D32" s="134"/>
+      <c r="E32" s="134"/>
+      <c r="F32" s="134"/>
+      <c r="G32" s="271"/>
+      <c r="H32" s="272"/>
+      <c r="I32" s="134"/>
+      <c r="J32" s="271"/>
+      <c r="K32" s="134"/>
+      <c r="L32" s="134"/>
+      <c r="M32" s="134"/>
+      <c r="N32" s="134"/>
+      <c r="O32" s="31">
+        <v>7</v>
+      </c>
+      <c r="P32" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q32" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="R32" s="32" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="247"/>
+      <c r="B33" s="247"/>
+      <c r="C33" s="134"/>
+      <c r="D33" s="134"/>
+      <c r="E33" s="134"/>
+      <c r="F33" s="134"/>
+      <c r="G33" s="271"/>
+      <c r="H33" s="272"/>
+      <c r="I33" s="134"/>
+      <c r="J33" s="271"/>
+      <c r="K33" s="134"/>
+      <c r="L33" s="134"/>
+      <c r="M33" s="134"/>
+      <c r="N33" s="134"/>
+      <c r="O33" s="31">
+        <v>8</v>
+      </c>
+      <c r="P33" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q33" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="R33" s="32" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="293" t="s">
+        <v>172</v>
+      </c>
+      <c r="B34" s="294"/>
+      <c r="C34" s="279" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="280"/>
+      <c r="E34" s="280"/>
+      <c r="F34" s="281"/>
+      <c r="G34" s="273" t="s">
+        <v>126</v>
+      </c>
+      <c r="H34" s="285" t="s">
+        <v>126</v>
+      </c>
+      <c r="I34" s="282" t="s">
+        <v>177</v>
+      </c>
+      <c r="J34" s="285" t="s">
+        <v>175</v>
+      </c>
+      <c r="K34" s="279" t="s">
+        <v>176</v>
+      </c>
+      <c r="L34" s="280"/>
+      <c r="M34" s="280"/>
+      <c r="N34" s="281"/>
+      <c r="O34" s="273"/>
+      <c r="P34" s="273"/>
+      <c r="Q34" s="273"/>
+      <c r="R34" s="273"/>
+    </row>
+    <row r="35" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="295" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" s="296"/>
+      <c r="C35" s="275" t="s">
+        <v>178</v>
+      </c>
+      <c r="D35" s="283"/>
+      <c r="E35" s="283"/>
+      <c r="F35" s="276"/>
+      <c r="G35" s="286" t="s">
+        <v>179</v>
+      </c>
+      <c r="H35" s="286" t="s">
+        <v>180</v>
+      </c>
+      <c r="I35" s="288" t="s">
+        <v>181</v>
+      </c>
+      <c r="J35" s="286"/>
+      <c r="K35" s="275"/>
+      <c r="L35" s="283"/>
+      <c r="M35" s="283"/>
+      <c r="N35" s="276"/>
+      <c r="O35" s="274">
+        <v>10</v>
+      </c>
+      <c r="P35" s="274" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q35" s="290" t="s">
+        <v>184</v>
+      </c>
+      <c r="R35" s="290" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="297"/>
+      <c r="B36" s="298"/>
+      <c r="C36" s="277"/>
+      <c r="D36" s="284"/>
+      <c r="E36" s="284"/>
+      <c r="F36" s="278"/>
+      <c r="G36" s="287"/>
+      <c r="H36" s="287"/>
+      <c r="I36" s="289"/>
+      <c r="J36" s="287"/>
+      <c r="K36" s="277"/>
+      <c r="L36" s="284"/>
+      <c r="M36" s="284"/>
+      <c r="N36" s="278"/>
+      <c r="O36" s="274">
+        <v>11</v>
+      </c>
+      <c r="P36" s="274" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q36" s="290" t="s">
+        <v>186</v>
+      </c>
+      <c r="R36" s="290" t="s">
+        <v>187</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="49">
+    <mergeCell ref="A35:B36"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F36"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="K35:N36"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="H27:H30"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="K27:N30"/>
+    <mergeCell ref="K24:N26"/>
     <mergeCell ref="Q18:R18"/>
     <mergeCell ref="A20:B23"/>
     <mergeCell ref="C20:F23"/>
@@ -3250,15 +4144,15 @@
     <mergeCell ref="I20:I23"/>
     <mergeCell ref="J20:J23"/>
     <mergeCell ref="K20:N23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="C27:F30"/>
+    <mergeCell ref="A27:B30"/>
+    <mergeCell ref="A31:B33"/>
+    <mergeCell ref="C31:F33"/>
+    <mergeCell ref="G31:G33"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="K31:N33"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
@@ -3269,24 +4163,39 @@
     <mergeCell ref="J18:N18"/>
     <mergeCell ref="O18:P18"/>
     <mergeCell ref="K19:N19"/>
+    <mergeCell ref="A24:B26"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="C24:F26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{47778F30-7A22-4070-8157-D398D2A3CE0F}"/>
-    <hyperlink ref="H26" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{D3F545D0-6E58-49FD-B848-5263BA70789A}"/>
-    <hyperlink ref="A24:B24" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{D4226CCC-5E80-4BCE-91C7-8796296A1724}"/>
-    <hyperlink ref="A26:B26" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{077D1BD0-B2E1-4C60-BE34-F7EFEE0BE80F}"/>
     <hyperlink ref="A1:P1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{A01559FD-0C7C-4112-A809-F49F4DACD93C}"/>
-    <hyperlink ref="A25:B25" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{8552B757-8DC3-490E-A26C-09AD5D9DDA62}"/>
     <hyperlink ref="B10" location="ObjetoDominio_Participante!A1" display="Participante" xr:uid="{65BE0D2A-5223-4BAE-A78D-FEF01705AAE1}"/>
     <hyperlink ref="B11" location="ObjetoDominio_ListaTarea!A1" display="ListaTareas" xr:uid="{4B321ACB-9E6C-44EE-95C8-0229FF27DA74}"/>
     <hyperlink ref="H20" location="ObjetoDominio_Proyectos!A1" display="Proyecto" xr:uid="{40CC0287-00F3-4ABE-A060-C8487E637CC8}"/>
-    <hyperlink ref="R4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{AB371578-E9ED-4E92-AAAC-6A9DAB3728CA}"/>
-    <hyperlink ref="S4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{A18C8F13-1F14-44DB-A0ED-D45BA28B04B6}"/>
-    <hyperlink ref="T4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{266F3904-D4CD-4A7F-9A48-5F780CAB7CD0}"/>
+    <hyperlink ref="R4" location="ObjetoDominio_Proyectos!A24" display="ObjetoDominio_Proyectos!A24" xr:uid="{AB371578-E9ED-4E92-AAAC-6A9DAB3728CA}"/>
+    <hyperlink ref="S4" location="ObjetoDominio_Proyectos!A27" display="ObjetoDominio_Proyectos!A27" xr:uid="{A18C8F13-1F14-44DB-A0ED-D45BA28B04B6}"/>
+    <hyperlink ref="T4" location="ObjetoDominio_Proyectos!A31" display="ObjetoDominio_Proyectos!A31" xr:uid="{266F3904-D4CD-4A7F-9A48-5F780CAB7CD0}"/>
     <hyperlink ref="Q4" location="ObjetoDominio_Proyectos!A20" display="ObjetoDominio_Proyectos!A20" xr:uid="{988D7633-97BF-4994-82C5-0CC5828A6983}"/>
     <hyperlink ref="A20:B23" location="ObjetoDominio_Proyectos!Q4" display="Crear" xr:uid="{FD470CAC-8EBE-4274-9F01-02F0EB28E4C2}"/>
+    <hyperlink ref="H31" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{D3F545D0-6E58-49FD-B848-5263BA70789A}"/>
+    <hyperlink ref="H20:H23" location="ObjetoDominio_Proyectos!A2" display="Proyecto" xr:uid="{118D705B-085D-4685-B284-3B26AA61824A}"/>
+    <hyperlink ref="H24" location="ObjetoDominio_Proyectos!A2" display="Proyecto" xr:uid="{DA3B397F-01CF-4F09-B0D0-D55E06F328A6}"/>
+    <hyperlink ref="A24:B26" location="ObjetoDominio_Proyectos!R4" display="ModificarNombreDescripcion" xr:uid="{15B80242-8768-45C0-8DF7-EFCFC07AC7B5}"/>
+    <hyperlink ref="H24:H26" location="ObjetoDominio_Proyectos!A2" display="Proyecto" xr:uid="{5EBC1402-2864-4417-8DB8-64F5A7433DA2}"/>
+    <hyperlink ref="H27:H30" location="ObjetoDominio_Proyectos!A2" display="Proyecto" xr:uid="{8A9BE81E-2F20-4244-9530-C97B156DD0BA}"/>
+    <hyperlink ref="H31:H33" location="ObjetoDominio_Proyectos!A2" display="Proyecto" xr:uid="{455EBACB-8A45-48FB-BC7B-F9AC6E4A0649}"/>
+    <hyperlink ref="U4" location="ObjetoDominio_Proyectos!A34" display="ObjetoDominio_Proyectos!A34" xr:uid="{34794B2D-3372-4FC7-9A52-AEEC405A4580}"/>
+    <hyperlink ref="V4" location="ObjetoDominio_Proyectos!A35" display="ObjetoDominio_Proyectos!A35" xr:uid="{3E90B945-6A49-4E65-A7C6-F5465DCC1458}"/>
+    <hyperlink ref="H34" location="ObjetoDominio_Proyectos!A2" display="Proyecto" xr:uid="{732B822F-3B83-4186-BB00-1D43B8C915F5}"/>
+    <hyperlink ref="J34" location="ObjetoDominio_Proyectos!A2" display="Proyecto" xr:uid="{04FEBAED-0D98-4CC7-B208-C2D98C9BCE8B}"/>
+    <hyperlink ref="A27:B30" location="ObjetoDominio_Proyectos!S4" display="ModificarFechaFinalizacion" xr:uid="{FBB3FABD-39BB-4EA9-A40B-69FE2EE62914}"/>
+    <hyperlink ref="A31:B33" location="ObjetoDominio_Proyectos!T4" display="ModificarParticipantes" xr:uid="{DE110AD2-9C6D-41C9-81EF-2BC935D17C7A}"/>
+    <hyperlink ref="A34:B34" location="ObjetoDominio_Proyectos!U4" display="Consultar" xr:uid="{79DA2B4D-6011-4E9C-9826-7139196C82F9}"/>
+    <hyperlink ref="A35:B36" location="ObjetoDominio_Proyectos!V4" display="Eliminar" xr:uid="{C7527E0C-11B7-48D6-9CF6-FFA6A8083195}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3295,7 +4204,7 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17:R22"/>
+      <selection activeCell="C20" sqref="C20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3325,70 +4234,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="106" t="str">
+      <c r="B2" s="114" t="str">
         <f>'Listado Objetos de Dominio'!$A$2</f>
         <v>ListaTareas</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
-      <c r="N2" s="106"/>
-      <c r="O2" s="106"/>
-      <c r="P2" s="106"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="114"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="114"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="107" t="str">
+      <c r="B3" s="115" t="str">
         <f>'Listado Objetos de Dominio'!$B$2</f>
         <v xml:space="preserve">Este objeto de dominio contiene  informacion de las listas de trabajo que tienen los proyectos </v>
       </c>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="115"/>
+      <c r="O3" s="115"/>
+      <c r="P3" s="115"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -3760,11 +4669,11 @@
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="108" t="s">
+      <c r="A13" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="109"/>
-      <c r="C13" s="110"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="118"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
@@ -3783,44 +4692,44 @@
       <c r="C15" s="38"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="111" t="s">
+      <c r="A17" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="112"/>
-      <c r="C17" s="112" t="s">
+      <c r="B17" s="120"/>
+      <c r="C17" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="112" t="s">
+      <c r="D17" s="120"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
+      <c r="G17" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="112"/>
-      <c r="I17" s="112"/>
-      <c r="J17" s="112" t="s">
+      <c r="H17" s="120"/>
+      <c r="I17" s="120"/>
+      <c r="J17" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="K17" s="112"/>
-      <c r="L17" s="112"/>
-      <c r="M17" s="112"/>
-      <c r="N17" s="112"/>
-      <c r="O17" s="112" t="s">
+      <c r="K17" s="120"/>
+      <c r="L17" s="120"/>
+      <c r="M17" s="120"/>
+      <c r="N17" s="120"/>
+      <c r="O17" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="112"/>
-      <c r="Q17" s="112" t="s">
+      <c r="P17" s="120"/>
+      <c r="Q17" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="R17" s="130"/>
+      <c r="R17" s="135"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="113"/>
-      <c r="B18" s="114"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114"/>
+      <c r="A18" s="121"/>
+      <c r="B18" s="122"/>
+      <c r="C18" s="122"/>
+      <c r="D18" s="122"/>
+      <c r="E18" s="122"/>
+      <c r="F18" s="122"/>
       <c r="G18" s="19" t="s">
         <v>28</v>
       </c>
@@ -3833,12 +4742,12 @@
       <c r="J18" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K18" s="114" t="s">
+      <c r="K18" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="L18" s="114"/>
-      <c r="M18" s="114"/>
-      <c r="N18" s="114"/>
+      <c r="L18" s="122"/>
+      <c r="M18" s="122"/>
+      <c r="N18" s="122"/>
       <c r="O18" s="19" t="s">
         <v>30</v>
       </c>
@@ -3853,16 +4762,16 @@
       </c>
     </row>
     <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="115" t="s">
+      <c r="A19" s="160" t="s">
         <v>136</v>
       </c>
-      <c r="B19" s="116"/>
-      <c r="C19" s="183" t="s">
+      <c r="B19" s="161"/>
+      <c r="C19" s="162" t="s">
         <v>137</v>
       </c>
-      <c r="D19" s="184"/>
-      <c r="E19" s="184"/>
-      <c r="F19" s="185"/>
+      <c r="D19" s="163"/>
+      <c r="E19" s="163"/>
+      <c r="F19" s="164"/>
       <c r="G19" s="20" t="s">
         <v>126</v>
       </c>
@@ -3871,76 +4780,76 @@
       </c>
       <c r="I19" s="22"/>
       <c r="J19" s="21"/>
-      <c r="K19" s="117"/>
-      <c r="L19" s="117"/>
-      <c r="M19" s="117"/>
-      <c r="N19" s="117"/>
+      <c r="K19" s="165"/>
+      <c r="L19" s="165"/>
+      <c r="M19" s="165"/>
+      <c r="N19" s="165"/>
       <c r="O19" s="20"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="26"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="118" t="s">
+      <c r="A20" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="119"/>
-      <c r="C20" s="186"/>
-      <c r="D20" s="187"/>
-      <c r="E20" s="187"/>
-      <c r="F20" s="188"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="109"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="111"/>
       <c r="G20" s="46"/>
       <c r="H20" s="44"/>
       <c r="I20" s="45"/>
       <c r="J20" s="39"/>
-      <c r="K20" s="121"/>
-      <c r="L20" s="121"/>
-      <c r="M20" s="121"/>
-      <c r="N20" s="121"/>
+      <c r="K20" s="112"/>
+      <c r="L20" s="112"/>
+      <c r="M20" s="112"/>
+      <c r="N20" s="112"/>
       <c r="O20" s="23"/>
       <c r="P20" s="24"/>
       <c r="Q20" s="24"/>
       <c r="R20" s="27"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="122" t="s">
+      <c r="A21" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="123"/>
-      <c r="C21" s="189"/>
-      <c r="D21" s="190"/>
-      <c r="E21" s="190"/>
-      <c r="F21" s="191"/>
+      <c r="B21" s="124"/>
+      <c r="C21" s="125"/>
+      <c r="D21" s="126"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="127"/>
       <c r="G21" s="42"/>
       <c r="H21" s="40"/>
       <c r="I21" s="41"/>
       <c r="J21" s="43"/>
-      <c r="K21" s="125"/>
-      <c r="L21" s="125"/>
-      <c r="M21" s="125"/>
-      <c r="N21" s="125"/>
+      <c r="K21" s="128"/>
+      <c r="L21" s="128"/>
+      <c r="M21" s="128"/>
+      <c r="N21" s="128"/>
       <c r="O21" s="28"/>
       <c r="P21" s="29"/>
       <c r="Q21" s="29"/>
       <c r="R21" s="30"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="126" t="s">
+      <c r="A22" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="127"/>
-      <c r="C22" s="192"/>
-      <c r="D22" s="193"/>
-      <c r="E22" s="193"/>
-      <c r="F22" s="194"/>
+      <c r="B22" s="130"/>
+      <c r="C22" s="131"/>
+      <c r="D22" s="132"/>
+      <c r="E22" s="132"/>
+      <c r="F22" s="133"/>
       <c r="G22" s="48"/>
       <c r="H22" s="49"/>
       <c r="I22" s="47"/>
       <c r="J22" s="48"/>
-      <c r="K22" s="129"/>
-      <c r="L22" s="129"/>
-      <c r="M22" s="129"/>
-      <c r="N22" s="129"/>
+      <c r="K22" s="134"/>
+      <c r="L22" s="134"/>
+      <c r="M22" s="134"/>
+      <c r="N22" s="134"/>
       <c r="O22" s="31"/>
       <c r="P22" s="32"/>
       <c r="Q22" s="32"/>
@@ -3997,7 +4906,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4027,70 +4936,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="106" t="str">
+      <c r="B2" s="114" t="str">
         <f>'Listado Objetos de Dominio'!$A$3</f>
         <v>Participante</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
-      <c r="N2" s="106"/>
-      <c r="O2" s="106"/>
-      <c r="P2" s="106"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="114"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="114"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="107" t="str">
+      <c r="B3" s="115" t="str">
         <f>'Listado Objetos de Dominio'!$B$3</f>
         <v xml:space="preserve">Este objeto de dominio me da la informacion de la persona que esta vinculada al proyecto </v>
       </c>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="115"/>
+      <c r="O3" s="115"/>
+      <c r="P3" s="115"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -4390,11 +5299,11 @@
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="108" t="s">
+      <c r="A11" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="109"/>
-      <c r="C11" s="110"/>
+      <c r="B11" s="117"/>
+      <c r="C11" s="118"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
@@ -4413,44 +5322,44 @@
       <c r="C13" s="38"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="111" t="s">
+      <c r="A15" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="112"/>
-      <c r="C15" s="112" t="s">
+      <c r="B15" s="120"/>
+      <c r="C15" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="112"/>
-      <c r="E15" s="112"/>
-      <c r="F15" s="112"/>
-      <c r="G15" s="112" t="s">
+      <c r="D15" s="120"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
+      <c r="G15" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="112"/>
-      <c r="I15" s="112"/>
-      <c r="J15" s="112" t="s">
+      <c r="H15" s="120"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="112"/>
-      <c r="L15" s="112"/>
-      <c r="M15" s="112"/>
-      <c r="N15" s="112"/>
-      <c r="O15" s="112" t="s">
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="120"/>
+      <c r="N15" s="120"/>
+      <c r="O15" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="112"/>
-      <c r="Q15" s="112" t="s">
+      <c r="P15" s="120"/>
+      <c r="Q15" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="R15" s="130"/>
+      <c r="R15" s="135"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="113"/>
-      <c r="B16" s="114"/>
-      <c r="C16" s="114"/>
-      <c r="D16" s="114"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
+      <c r="A16" s="121"/>
+      <c r="B16" s="122"/>
+      <c r="C16" s="122"/>
+      <c r="D16" s="122"/>
+      <c r="E16" s="122"/>
+      <c r="F16" s="122"/>
       <c r="G16" s="19" t="s">
         <v>28</v>
       </c>
@@ -4463,12 +5372,12 @@
       <c r="J16" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="114" t="s">
+      <c r="K16" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="L16" s="114"/>
-      <c r="M16" s="114"/>
-      <c r="N16" s="114"/>
+      <c r="L16" s="122"/>
+      <c r="M16" s="122"/>
+      <c r="N16" s="122"/>
       <c r="O16" s="19" t="s">
         <v>30</v>
       </c>
@@ -4483,88 +5392,88 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="115" t="s">
+      <c r="A17" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="116"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
+      <c r="B17" s="161"/>
+      <c r="C17" s="165"/>
+      <c r="D17" s="165"/>
+      <c r="E17" s="165"/>
+      <c r="F17" s="165"/>
       <c r="G17" s="20"/>
       <c r="H17" s="21"/>
       <c r="I17" s="22"/>
       <c r="J17" s="21"/>
-      <c r="K17" s="117"/>
-      <c r="L17" s="117"/>
-      <c r="M17" s="117"/>
-      <c r="N17" s="117"/>
+      <c r="K17" s="165"/>
+      <c r="L17" s="165"/>
+      <c r="M17" s="165"/>
+      <c r="N17" s="165"/>
       <c r="O17" s="20"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="26"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="118" t="s">
+      <c r="A18" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="119"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
+      <c r="B18" s="108"/>
+      <c r="C18" s="168"/>
+      <c r="D18" s="168"/>
+      <c r="E18" s="168"/>
+      <c r="F18" s="168"/>
       <c r="G18" s="46"/>
       <c r="H18" s="44"/>
       <c r="I18" s="45"/>
       <c r="J18" s="39"/>
-      <c r="K18" s="121"/>
-      <c r="L18" s="121"/>
-      <c r="M18" s="121"/>
-      <c r="N18" s="121"/>
+      <c r="K18" s="112"/>
+      <c r="L18" s="112"/>
+      <c r="M18" s="112"/>
+      <c r="N18" s="112"/>
       <c r="O18" s="23"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
       <c r="R18" s="27"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="122" t="s">
+      <c r="A19" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="123"/>
-      <c r="C19" s="124"/>
-      <c r="D19" s="124"/>
-      <c r="E19" s="124"/>
-      <c r="F19" s="124"/>
+      <c r="B19" s="124"/>
+      <c r="C19" s="166"/>
+      <c r="D19" s="166"/>
+      <c r="E19" s="166"/>
+      <c r="F19" s="166"/>
       <c r="G19" s="42"/>
       <c r="H19" s="40"/>
       <c r="I19" s="41"/>
       <c r="J19" s="43"/>
-      <c r="K19" s="125"/>
-      <c r="L19" s="125"/>
-      <c r="M19" s="125"/>
-      <c r="N19" s="125"/>
+      <c r="K19" s="128"/>
+      <c r="L19" s="128"/>
+      <c r="M19" s="128"/>
+      <c r="N19" s="128"/>
       <c r="O19" s="28"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="29"/>
       <c r="R19" s="30"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="126" t="s">
+      <c r="A20" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="127"/>
-      <c r="C20" s="128"/>
-      <c r="D20" s="128"/>
-      <c r="E20" s="128"/>
-      <c r="F20" s="128"/>
+      <c r="B20" s="130"/>
+      <c r="C20" s="167"/>
+      <c r="D20" s="167"/>
+      <c r="E20" s="167"/>
+      <c r="F20" s="167"/>
       <c r="G20" s="48"/>
       <c r="H20" s="49"/>
       <c r="I20" s="47"/>
       <c r="J20" s="48"/>
-      <c r="K20" s="129"/>
-      <c r="L20" s="129"/>
-      <c r="M20" s="129"/>
-      <c r="N20" s="129"/>
+      <c r="K20" s="134"/>
+      <c r="L20" s="134"/>
+      <c r="M20" s="134"/>
+      <c r="N20" s="134"/>
       <c r="O20" s="31"/>
       <c r="P20" s="32"/>
       <c r="Q20" s="32"/>
@@ -4635,24 +5544,24 @@
       <c r="A1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="136" t="str">
+      <c r="B1" s="174" t="str">
         <f>'Listado Objetos de Dominio'!$A$7</f>
         <v>MetricaProyecto</v>
       </c>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="137"/>
-      <c r="M1" s="137"/>
-      <c r="N1" s="137"/>
-      <c r="O1" s="137"/>
-      <c r="P1" s="138"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="175"/>
+      <c r="I1" s="175"/>
+      <c r="J1" s="175"/>
+      <c r="K1" s="175"/>
+      <c r="L1" s="175"/>
+      <c r="M1" s="175"/>
+      <c r="N1" s="175"/>
+      <c r="O1" s="175"/>
+      <c r="P1" s="176"/>
       <c r="Q1" s="57"/>
       <c r="R1" s="57"/>
       <c r="S1" s="57"/>
@@ -4662,24 +5571,24 @@
       <c r="A2" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="133" t="str">
+      <c r="B2" s="171" t="str">
         <f>'Listado Objetos de Dominio'!$B$7</f>
         <v>Objeto de dominio que contiene los datos necesarios para realizar el analisis estadistico a proyecto</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="134"/>
-      <c r="O2" s="134"/>
-      <c r="P2" s="135"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
+      <c r="F2" s="172"/>
+      <c r="G2" s="172"/>
+      <c r="H2" s="172"/>
+      <c r="I2" s="172"/>
+      <c r="J2" s="172"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="172"/>
+      <c r="M2" s="172"/>
+      <c r="N2" s="172"/>
+      <c r="O2" s="172"/>
+      <c r="P2" s="173"/>
       <c r="Q2" s="57"/>
       <c r="R2" s="57"/>
       <c r="S2" s="57"/>
@@ -5046,11 +5955,11 @@
       <c r="T10" s="57"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="155" t="s">
+      <c r="A11" s="193" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="156"/>
-      <c r="C11" s="157"/>
+      <c r="B11" s="194"/>
+      <c r="C11" s="195"/>
       <c r="D11" s="57"/>
       <c r="E11" s="57"/>
       <c r="F11" s="57"/>
@@ -5152,46 +6061,46 @@
       <c r="T14" s="57"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="158" t="s">
+      <c r="A15" s="196" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="159"/>
-      <c r="C15" s="162" t="s">
+      <c r="B15" s="197"/>
+      <c r="C15" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="163"/>
-      <c r="E15" s="163"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="131" t="s">
+      <c r="D15" s="201"/>
+      <c r="E15" s="201"/>
+      <c r="F15" s="197"/>
+      <c r="G15" s="169" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="166"/>
-      <c r="I15" s="132"/>
-      <c r="J15" s="131" t="s">
+      <c r="H15" s="204"/>
+      <c r="I15" s="170"/>
+      <c r="J15" s="169" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="166"/>
-      <c r="L15" s="166"/>
-      <c r="M15" s="166"/>
-      <c r="N15" s="132"/>
-      <c r="O15" s="131" t="s">
+      <c r="K15" s="204"/>
+      <c r="L15" s="204"/>
+      <c r="M15" s="204"/>
+      <c r="N15" s="170"/>
+      <c r="O15" s="169" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="132"/>
-      <c r="Q15" s="131" t="s">
+      <c r="P15" s="170"/>
+      <c r="Q15" s="169" t="s">
         <v>27</v>
       </c>
-      <c r="R15" s="132"/>
+      <c r="R15" s="170"/>
       <c r="S15" s="57"/>
       <c r="T15" s="57"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="160"/>
-      <c r="B16" s="161"/>
-      <c r="C16" s="164"/>
-      <c r="D16" s="165"/>
-      <c r="E16" s="165"/>
-      <c r="F16" s="161"/>
+      <c r="A16" s="198"/>
+      <c r="B16" s="199"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="203"/>
+      <c r="E16" s="203"/>
+      <c r="F16" s="199"/>
       <c r="G16" s="79" t="s">
         <v>28</v>
       </c>
@@ -5204,12 +6113,12 @@
       <c r="J16" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="175" t="s">
+      <c r="K16" s="213" t="s">
         <v>1</v>
       </c>
-      <c r="L16" s="176"/>
-      <c r="M16" s="176"/>
-      <c r="N16" s="177"/>
+      <c r="L16" s="214"/>
+      <c r="M16" s="214"/>
+      <c r="N16" s="215"/>
       <c r="O16" s="79" t="s">
         <v>30</v>
       </c>
@@ -5226,22 +6135,22 @@
       <c r="T16" s="57"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="178" t="s">
+      <c r="A17" s="216" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="179"/>
-      <c r="C17" s="180"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="181"/>
-      <c r="F17" s="182"/>
+      <c r="B17" s="217"/>
+      <c r="C17" s="218"/>
+      <c r="D17" s="219"/>
+      <c r="E17" s="219"/>
+      <c r="F17" s="220"/>
       <c r="G17" s="81"/>
       <c r="H17" s="82"/>
       <c r="I17" s="83"/>
       <c r="J17" s="82"/>
-      <c r="K17" s="180"/>
-      <c r="L17" s="181"/>
-      <c r="M17" s="181"/>
-      <c r="N17" s="182"/>
+      <c r="K17" s="218"/>
+      <c r="L17" s="219"/>
+      <c r="M17" s="219"/>
+      <c r="N17" s="220"/>
       <c r="O17" s="81"/>
       <c r="P17" s="81"/>
       <c r="Q17" s="81"/>
@@ -5250,22 +6159,22 @@
       <c r="T17" s="57"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="139" t="s">
+      <c r="A18" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="140"/>
-      <c r="C18" s="141"/>
-      <c r="D18" s="142"/>
-      <c r="E18" s="142"/>
-      <c r="F18" s="143"/>
+      <c r="B18" s="178"/>
+      <c r="C18" s="179"/>
+      <c r="D18" s="180"/>
+      <c r="E18" s="180"/>
+      <c r="F18" s="181"/>
       <c r="G18" s="85"/>
       <c r="H18" s="86"/>
       <c r="I18" s="87"/>
       <c r="J18" s="88"/>
-      <c r="K18" s="144"/>
-      <c r="L18" s="145"/>
-      <c r="M18" s="145"/>
-      <c r="N18" s="146"/>
+      <c r="K18" s="182"/>
+      <c r="L18" s="183"/>
+      <c r="M18" s="183"/>
+      <c r="N18" s="184"/>
       <c r="O18" s="70"/>
       <c r="P18" s="89"/>
       <c r="Q18" s="89"/>
@@ -5274,22 +6183,22 @@
       <c r="T18" s="57"/>
     </row>
     <row r="19" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="167" t="s">
+      <c r="A19" s="205" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="168"/>
-      <c r="C19" s="169"/>
-      <c r="D19" s="170"/>
-      <c r="E19" s="170"/>
-      <c r="F19" s="171"/>
+      <c r="B19" s="206"/>
+      <c r="C19" s="207"/>
+      <c r="D19" s="208"/>
+      <c r="E19" s="208"/>
+      <c r="F19" s="209"/>
       <c r="G19" s="91"/>
       <c r="H19" s="92"/>
       <c r="I19" s="93"/>
       <c r="J19" s="94"/>
-      <c r="K19" s="172"/>
-      <c r="L19" s="173"/>
-      <c r="M19" s="173"/>
-      <c r="N19" s="174"/>
+      <c r="K19" s="210"/>
+      <c r="L19" s="211"/>
+      <c r="M19" s="211"/>
+      <c r="N19" s="212"/>
       <c r="O19" s="71"/>
       <c r="P19" s="95"/>
       <c r="Q19" s="95"/>
@@ -5298,22 +6207,22 @@
       <c r="T19" s="57"/>
     </row>
     <row r="20" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="147" t="s">
+      <c r="A20" s="185" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="148"/>
-      <c r="C20" s="149"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="151"/>
+      <c r="B20" s="186"/>
+      <c r="C20" s="187"/>
+      <c r="D20" s="188"/>
+      <c r="E20" s="188"/>
+      <c r="F20" s="189"/>
       <c r="G20" s="97"/>
       <c r="H20" s="98"/>
       <c r="I20" s="99"/>
       <c r="J20" s="97"/>
-      <c r="K20" s="152"/>
-      <c r="L20" s="153"/>
-      <c r="M20" s="153"/>
-      <c r="N20" s="154"/>
+      <c r="K20" s="190"/>
+      <c r="L20" s="191"/>
+      <c r="M20" s="191"/>
+      <c r="N20" s="192"/>
       <c r="O20" s="72"/>
       <c r="P20" s="100"/>
       <c r="Q20" s="100"/>
@@ -5400,70 +6309,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="106" t="str">
+      <c r="B2" s="114" t="str">
         <f>'Listado Objetos de Dominio'!$A$4</f>
         <v>Tarea</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
-      <c r="N2" s="106"/>
-      <c r="O2" s="106"/>
-      <c r="P2" s="106"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="114"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="114"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="107" t="str">
+      <c r="B3" s="115" t="str">
         <f>'Listado Objetos de Dominio'!$B$4</f>
         <v>Este objeto de dominio contiene la información de una tarea que esta dentro de una listaTarea</v>
       </c>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="115"/>
+      <c r="O3" s="115"/>
+      <c r="P3" s="115"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -5863,44 +6772,44 @@
     </row>
     <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="111" t="s">
+      <c r="A14" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="112"/>
-      <c r="C14" s="112" t="s">
+      <c r="B14" s="120"/>
+      <c r="C14" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="112"/>
-      <c r="E14" s="112"/>
-      <c r="F14" s="112"/>
-      <c r="G14" s="112" t="s">
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="112"/>
-      <c r="I14" s="112"/>
-      <c r="J14" s="112" t="s">
+      <c r="H14" s="120"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="112"/>
-      <c r="L14" s="112"/>
-      <c r="M14" s="112"/>
-      <c r="N14" s="112"/>
-      <c r="O14" s="112" t="s">
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="120"/>
+      <c r="O14" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="112"/>
-      <c r="Q14" s="112" t="s">
+      <c r="P14" s="120"/>
+      <c r="Q14" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="R14" s="130"/>
+      <c r="R14" s="135"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="113"/>
-      <c r="B15" s="114"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="114"/>
-      <c r="F15" s="114"/>
+      <c r="A15" s="121"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="122"/>
+      <c r="D15" s="122"/>
+      <c r="E15" s="122"/>
+      <c r="F15" s="122"/>
       <c r="G15" s="19" t="s">
         <v>28</v>
       </c>
@@ -5913,12 +6822,12 @@
       <c r="J15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="114" t="s">
+      <c r="K15" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="L15" s="114"/>
-      <c r="M15" s="114"/>
-      <c r="N15" s="114"/>
+      <c r="L15" s="122"/>
+      <c r="M15" s="122"/>
+      <c r="N15" s="122"/>
       <c r="O15" s="19" t="s">
         <v>30</v>
       </c>
@@ -5933,88 +6842,88 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="115" t="s">
+      <c r="A16" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="116"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="B16" s="161"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
       <c r="G16" s="20"/>
       <c r="H16" s="21"/>
       <c r="I16" s="22"/>
       <c r="J16" s="21"/>
-      <c r="K16" s="117"/>
-      <c r="L16" s="117"/>
-      <c r="M16" s="117"/>
-      <c r="N16" s="117"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
+      <c r="M16" s="165"/>
+      <c r="N16" s="165"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="20"/>
       <c r="R16" s="26"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="118" t="s">
+      <c r="A17" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="119"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="168"/>
+      <c r="D17" s="168"/>
+      <c r="E17" s="168"/>
+      <c r="F17" s="168"/>
       <c r="G17" s="46"/>
       <c r="H17" s="44"/>
       <c r="I17" s="45"/>
       <c r="J17" s="39"/>
-      <c r="K17" s="121"/>
-      <c r="L17" s="121"/>
-      <c r="M17" s="121"/>
-      <c r="N17" s="121"/>
+      <c r="K17" s="112"/>
+      <c r="L17" s="112"/>
+      <c r="M17" s="112"/>
+      <c r="N17" s="112"/>
       <c r="O17" s="23"/>
       <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
       <c r="R17" s="27"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="122" t="s">
+      <c r="A18" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="123"/>
-      <c r="C18" s="124"/>
-      <c r="D18" s="124"/>
-      <c r="E18" s="124"/>
-      <c r="F18" s="124"/>
+      <c r="B18" s="124"/>
+      <c r="C18" s="166"/>
+      <c r="D18" s="166"/>
+      <c r="E18" s="166"/>
+      <c r="F18" s="166"/>
       <c r="G18" s="42"/>
       <c r="H18" s="40"/>
       <c r="I18" s="41"/>
       <c r="J18" s="43"/>
-      <c r="K18" s="125"/>
-      <c r="L18" s="125"/>
-      <c r="M18" s="125"/>
-      <c r="N18" s="125"/>
+      <c r="K18" s="128"/>
+      <c r="L18" s="128"/>
+      <c r="M18" s="128"/>
+      <c r="N18" s="128"/>
       <c r="O18" s="28"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="29"/>
       <c r="R18" s="30"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="126" t="s">
+      <c r="A19" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="127"/>
-      <c r="C19" s="128"/>
-      <c r="D19" s="128"/>
-      <c r="E19" s="128"/>
-      <c r="F19" s="128"/>
+      <c r="B19" s="130"/>
+      <c r="C19" s="167"/>
+      <c r="D19" s="167"/>
+      <c r="E19" s="167"/>
+      <c r="F19" s="167"/>
       <c r="G19" s="48"/>
       <c r="H19" s="49"/>
       <c r="I19" s="47"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="129"/>
-      <c r="L19" s="129"/>
-      <c r="M19" s="129"/>
-      <c r="N19" s="129"/>
+      <c r="K19" s="134"/>
+      <c r="L19" s="134"/>
+      <c r="M19" s="134"/>
+      <c r="N19" s="134"/>
       <c r="O19" s="31"/>
       <c r="P19" s="32"/>
       <c r="Q19" s="32"/>
@@ -6099,70 +7008,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="106" t="str">
+      <c r="B2" s="114" t="str">
         <f>'Listado Objetos de Dominio'!$A$5</f>
         <v>Estado</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
-      <c r="N2" s="106"/>
-      <c r="O2" s="106"/>
-      <c r="P2" s="106"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="114"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="114"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="107" t="str">
+      <c r="B3" s="115" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v>Este objeto de dominio contiene el estado de realización en el que puede estar una lista de tareas o una tarea</v>
       </c>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="115"/>
+      <c r="O3" s="115"/>
+      <c r="P3" s="115"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -6324,44 +7233,44 @@
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="111" t="s">
+      <c r="A8" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="112"/>
-      <c r="C8" s="112" t="s">
+      <c r="B8" s="120"/>
+      <c r="C8" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112" t="s">
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="112"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="112" t="s">
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="112"/>
-      <c r="L8" s="112"/>
-      <c r="M8" s="112"/>
-      <c r="N8" s="112"/>
-      <c r="O8" s="112" t="s">
+      <c r="K8" s="120"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="120"/>
+      <c r="N8" s="120"/>
+      <c r="O8" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="P8" s="112"/>
-      <c r="Q8" s="112" t="s">
+      <c r="P8" s="120"/>
+      <c r="Q8" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="130"/>
+      <c r="R8" s="135"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="113"/>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
+      <c r="A9" s="121"/>
+      <c r="B9" s="122"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
       <c r="G9" s="19" t="s">
         <v>28</v>
       </c>
@@ -6374,12 +7283,12 @@
       <c r="J9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="114" t="s">
+      <c r="K9" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="114"/>
-      <c r="M9" s="114"/>
-      <c r="N9" s="114"/>
+      <c r="L9" s="122"/>
+      <c r="M9" s="122"/>
+      <c r="N9" s="122"/>
       <c r="O9" s="19" t="s">
         <v>30</v>
       </c>
@@ -6394,88 +7303,88 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="115" t="s">
+      <c r="A10" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="116"/>
-      <c r="C10" s="117"/>
-      <c r="D10" s="117"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="117"/>
+      <c r="B10" s="161"/>
+      <c r="C10" s="165"/>
+      <c r="D10" s="165"/>
+      <c r="E10" s="165"/>
+      <c r="F10" s="165"/>
       <c r="G10" s="20"/>
       <c r="H10" s="21"/>
       <c r="I10" s="22"/>
       <c r="J10" s="21"/>
-      <c r="K10" s="117"/>
-      <c r="L10" s="117"/>
-      <c r="M10" s="117"/>
-      <c r="N10" s="117"/>
+      <c r="K10" s="165"/>
+      <c r="L10" s="165"/>
+      <c r="M10" s="165"/>
+      <c r="N10" s="165"/>
       <c r="O10" s="20"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="26"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="119"/>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="168"/>
+      <c r="D11" s="168"/>
+      <c r="E11" s="168"/>
+      <c r="F11" s="168"/>
       <c r="G11" s="46"/>
       <c r="H11" s="44"/>
       <c r="I11" s="45"/>
       <c r="J11" s="39"/>
-      <c r="K11" s="121"/>
-      <c r="L11" s="121"/>
-      <c r="M11" s="121"/>
-      <c r="N11" s="121"/>
+      <c r="K11" s="112"/>
+      <c r="L11" s="112"/>
+      <c r="M11" s="112"/>
+      <c r="N11" s="112"/>
       <c r="O11" s="23"/>
       <c r="P11" s="24"/>
       <c r="Q11" s="24"/>
       <c r="R11" s="27"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="122" t="s">
+      <c r="A12" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="123"/>
-      <c r="C12" s="124"/>
-      <c r="D12" s="124"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="124"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="166"/>
+      <c r="E12" s="166"/>
+      <c r="F12" s="166"/>
       <c r="G12" s="42"/>
       <c r="H12" s="40"/>
       <c r="I12" s="41"/>
       <c r="J12" s="43"/>
-      <c r="K12" s="125"/>
-      <c r="L12" s="125"/>
-      <c r="M12" s="125"/>
-      <c r="N12" s="125"/>
+      <c r="K12" s="128"/>
+      <c r="L12" s="128"/>
+      <c r="M12" s="128"/>
+      <c r="N12" s="128"/>
       <c r="O12" s="28"/>
       <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
       <c r="R12" s="30"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="126" t="s">
+      <c r="A13" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="127"/>
-      <c r="C13" s="128"/>
-      <c r="D13" s="128"/>
-      <c r="E13" s="128"/>
-      <c r="F13" s="128"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="167"/>
+      <c r="D13" s="167"/>
+      <c r="E13" s="167"/>
+      <c r="F13" s="167"/>
       <c r="G13" s="48"/>
       <c r="H13" s="49"/>
       <c r="I13" s="47"/>
       <c r="J13" s="48"/>
-      <c r="K13" s="129"/>
-      <c r="L13" s="129"/>
-      <c r="M13" s="129"/>
-      <c r="N13" s="129"/>
+      <c r="K13" s="134"/>
+      <c r="L13" s="134"/>
+      <c r="M13" s="134"/>
+      <c r="N13" s="134"/>
       <c r="O13" s="31"/>
       <c r="P13" s="32"/>
       <c r="Q13" s="32"/>
@@ -6525,6 +7434,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6533,7 +7448,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001D0DE5568C0AE848B2F225150E15E78E" ma:contentTypeVersion="3" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="643d399a24376eab49db33c80db032ac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="915fd109-ae29-4648-8de1-7f064f1d0fe5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2a54904d818499acdea7742e4a0622bc" ns2:_="">
     <xsd:import namespace="915fd109-ae29-4648-8de1-7f064f1d0fe5"/>
@@ -6671,13 +7586,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -6685,7 +7603,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C779E5F7-74AC-4CCB-8FB1-CBA1DF721FBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6703,15 +7621,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{86cab09b-e61a-4c01-96e7-67fc9e3d8cd5}" enabled="1" method="Standard" siteId="{bf1ce8b5-5d39-4bc5-ad6e-07b3e4d7d67a}" contentBits="8" removed="0"/>

</xml_diff>